<commit_message>
platform stm32f4: update pin mappings
</commit_message>
<xml_diff>
--- a/platform/embedded/stm32f407/stm32f4_function_mappings.xlsx
+++ b/platform/embedded/stm32f407/stm32f4_function_mappings.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2402" uniqueCount="419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2405" uniqueCount="422">
   <si>
     <t xml:space="preserve">Port</t>
   </si>
@@ -809,10 +809,19 @@
     <t xml:space="preserve">PC13</t>
   </si>
   <si>
+    <t xml:space="preserve">NRF_CE</t>
+  </si>
+  <si>
     <t xml:space="preserve">PC14</t>
   </si>
   <si>
+    <t xml:space="preserve">NRF_CSN</t>
+  </si>
+  <si>
     <t xml:space="preserve">PC15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NRF_IRQ</t>
   </si>
   <si>
     <t xml:space="preserve">PD0</t>
@@ -1378,7 +1387,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1407,6 +1416,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFF33FF"/>
         <bgColor rgb="FFFF00FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B274"/>
+        <bgColor rgb="FF008080"/>
       </patternFill>
     </fill>
     <fill>
@@ -1456,7 +1471,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="42">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1569,12 +1584,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1585,16 +1596,12 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1605,8 +1612,32 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1669,7 +1700,7 @@
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF00B274"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF993300"/>
@@ -1686,32 +1717,32 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q142"/>
+  <dimension ref="A1:R142"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="K36" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
-      <selection pane="bottomRight" activeCell="I22" activeCellId="0" sqref="I22"/>
+      <selection pane="topRight" activeCell="K1" activeCellId="0" sqref="K1"/>
+      <selection pane="bottomLeft" activeCell="A36" activeCellId="0" sqref="A36"/>
+      <selection pane="bottomRight" activeCell="R49" activeCellId="0" sqref="R49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="14.1020408163265"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.265306122449"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.7040816326531"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="8.36734693877551"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="12.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="10.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="14.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="15.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="13.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="12.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="16" style="0" width="8.37"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4028,7 +4059,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="25.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="24" t="s">
         <v>233</v>
       </c>
@@ -4103,7 +4134,7 @@
       <c r="G46" s="25" t="s">
         <v>135</v>
       </c>
-      <c r="H46" s="25" t="s">
+      <c r="H46" s="26" t="s">
         <v>134</v>
       </c>
       <c r="I46" s="25" t="s">
@@ -4134,7 +4165,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="25.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="24" t="s">
         <v>240</v>
       </c>
@@ -4187,274 +4218,283 @@
         <v>32</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="5" t="s">
+    <row r="48" s="32" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="29" t="s">
         <v>244</v>
       </c>
-      <c r="B48" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C48" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D48" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E48" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F48" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G48" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="H48" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="I48" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="J48" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="K48" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="L48" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="M48" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="N48" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="O48" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="P48" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q48" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="5" t="s">
+      <c r="B48" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="C48" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="D48" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="E48" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="F48" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="G48" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="H48" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="I48" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="J48" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="K48" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="L48" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="M48" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="N48" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="O48" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="P48" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q48" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="R48" s="32" t="s">
         <v>245</v>
       </c>
-      <c r="B49" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C49" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D49" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E49" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F49" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G49" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="H49" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="I49" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="J49" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="K49" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="L49" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="M49" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="N49" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="O49" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="P49" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q49" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="5" t="s">
+    </row>
+    <row r="49" s="32" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="29" t="s">
         <v>246</v>
       </c>
-      <c r="B50" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C50" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D50" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E50" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F50" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G50" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="H50" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="I50" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="J50" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="K50" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="L50" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="M50" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="N50" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="O50" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="P50" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q50" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="51" s="33" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="30" t="s">
+      <c r="B49" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="C49" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="D49" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="E49" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="F49" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="G49" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="H49" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="I49" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="J49" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="K49" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="L49" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="M49" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="N49" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="O49" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="P49" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q49" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="R49" s="32" t="s">
         <v>247</v>
       </c>
-      <c r="B51" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="C51" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="D51" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="E51" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="F51" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="G51" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="H51" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="I51" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="J51" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="K51" s="31" t="s">
+    </row>
+    <row r="50" s="32" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="29" t="s">
+        <v>248</v>
+      </c>
+      <c r="B50" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="C50" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="D50" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="E50" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="F50" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="G50" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="H50" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="I50" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="J50" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="K50" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="L50" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="M50" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="N50" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="O50" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="P50" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q50" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="R50" s="32" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="51" s="36" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="33" t="s">
+        <v>250</v>
+      </c>
+      <c r="B51" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="C51" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="D51" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="E51" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="F51" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="G51" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="H51" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="I51" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="J51" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="K51" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="L51" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="M51" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="N51" s="32" t="s">
-        <v>248</v>
-      </c>
-      <c r="O51" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="P51" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q51" s="31" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="52" s="33" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="30" t="s">
-        <v>249</v>
-      </c>
-      <c r="B52" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="C52" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="D52" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="E52" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="F52" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="G52" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="H52" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="I52" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="J52" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="K52" s="31" t="s">
+      <c r="L51" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="M51" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="N51" s="35" t="s">
+        <v>251</v>
+      </c>
+      <c r="O51" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="P51" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q51" s="34" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="52" s="36" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="33" t="s">
+        <v>252</v>
+      </c>
+      <c r="B52" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="C52" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="D52" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="E52" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="F52" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="G52" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="H52" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="I52" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="J52" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="K52" s="34" t="s">
         <v>106</v>
       </c>
-      <c r="L52" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="M52" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="N52" s="32" t="s">
-        <v>250</v>
-      </c>
-      <c r="O52" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="P52" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q52" s="31" t="s">
+      <c r="L52" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="M52" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="N52" s="35" t="s">
+        <v>253</v>
+      </c>
+      <c r="O52" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="P52" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q52" s="34" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="53" s="27" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="24" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="B53" s="25" t="s">
         <v>32</v>
@@ -4463,7 +4503,7 @@
         <v>32</v>
       </c>
       <c r="D53" s="25" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="E53" s="25" t="s">
         <v>32</v>
@@ -4481,7 +4521,7 @@
         <v>32</v>
       </c>
       <c r="J53" s="25" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="K53" s="25" t="s">
         <v>32</v>
@@ -4493,10 +4533,10 @@
         <v>32</v>
       </c>
       <c r="N53" s="26" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="O53" s="25" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="P53" s="25" t="s">
         <v>32</v>
@@ -4507,7 +4547,7 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="5" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="B54" s="6" t="s">
         <v>32</v>
@@ -4546,7 +4586,7 @@
         <v>32</v>
       </c>
       <c r="N54" s="6" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="O54" s="6" t="s">
         <v>32</v>
@@ -4558,115 +4598,115 @@
         <v>32</v>
       </c>
     </row>
-    <row r="55" s="33" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="B55" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="C55" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="D55" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="E55" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="F55" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="G55" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="H55" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="I55" s="31" t="s">
+    <row r="55" s="36" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="33" t="s">
+        <v>261</v>
+      </c>
+      <c r="B55" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="C55" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="D55" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="E55" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="F55" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="G55" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="H55" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="I55" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="J55" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="K55" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="L55" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="M55" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="N55" s="32" t="s">
-        <v>259</v>
-      </c>
-      <c r="O55" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="P55" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q55" s="31" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="56" s="33" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="30" t="s">
-        <v>260</v>
-      </c>
-      <c r="B56" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="C56" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="D56" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="E56" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="F56" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="G56" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="H56" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="I56" s="31" t="s">
+      <c r="J55" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="K55" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="L55" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="M55" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="N55" s="35" t="s">
+        <v>262</v>
+      </c>
+      <c r="O55" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="P55" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q55" s="34" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="56" s="36" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="33" t="s">
+        <v>263</v>
+      </c>
+      <c r="B56" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="C56" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="D56" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="E56" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="F56" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="G56" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="H56" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="I56" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="J56" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="K56" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="L56" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="M56" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="N56" s="32" t="s">
-        <v>261</v>
-      </c>
-      <c r="O56" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="P56" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q56" s="31" t="s">
+      <c r="J56" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="K56" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="L56" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="M56" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="N56" s="35" t="s">
+        <v>264</v>
+      </c>
+      <c r="O56" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="P56" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q56" s="34" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="5" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="B57" s="6" t="s">
         <v>32</v>
@@ -4705,7 +4745,7 @@
         <v>32</v>
       </c>
       <c r="N57" s="6" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="O57" s="6" t="s">
         <v>32</v>
@@ -4717,486 +4757,486 @@
         <v>32</v>
       </c>
     </row>
-    <row r="58" s="33" customFormat="true" ht="25.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="30" t="s">
-        <v>264</v>
-      </c>
-      <c r="B58" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="C58" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="D58" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="E58" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="F58" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="G58" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="H58" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="I58" s="31" t="s">
+    <row r="58" s="36" customFormat="true" ht="25.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="33" t="s">
+        <v>267</v>
+      </c>
+      <c r="B58" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="C58" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="D58" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="E58" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="F58" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="G58" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="H58" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="I58" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="J58" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="K58" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="L58" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="M58" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="N58" s="34" t="s">
-        <v>265</v>
-      </c>
-      <c r="O58" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="P58" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q58" s="31" t="s">
+      <c r="J58" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="K58" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="L58" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="M58" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="N58" s="37" t="s">
+        <v>268</v>
+      </c>
+      <c r="O58" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="P58" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q58" s="34" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="30" t="s">
-        <v>266</v>
-      </c>
-      <c r="B59" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="C59" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="D59" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="E59" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="F59" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="G59" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="H59" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="I59" s="31" t="s">
+      <c r="A59" s="33" t="s">
+        <v>269</v>
+      </c>
+      <c r="B59" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="C59" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="D59" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="E59" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="F59" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="G59" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="H59" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="I59" s="34" t="s">
         <v>168</v>
       </c>
-      <c r="J59" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="K59" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="L59" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="M59" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="N59" s="32" t="s">
-        <v>267</v>
-      </c>
-      <c r="O59" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="P59" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q59" s="31" t="s">
+      <c r="J59" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="K59" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="L59" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="M59" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="N59" s="35" t="s">
+        <v>270</v>
+      </c>
+      <c r="O59" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="P59" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q59" s="34" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="30" t="s">
-        <v>268</v>
-      </c>
-      <c r="B60" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="C60" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="D60" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="E60" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="F60" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="G60" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="H60" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="I60" s="31" t="s">
+      <c r="A60" s="33" t="s">
+        <v>271</v>
+      </c>
+      <c r="B60" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="C60" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="D60" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="E60" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="F60" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="G60" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="H60" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="I60" s="34" t="s">
         <v>173</v>
       </c>
-      <c r="J60" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="K60" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="L60" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="M60" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="N60" s="32" t="s">
-        <v>269</v>
-      </c>
-      <c r="O60" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="P60" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q60" s="31" t="s">
+      <c r="J60" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="K60" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="L60" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="M60" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="N60" s="35" t="s">
+        <v>272</v>
+      </c>
+      <c r="O60" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="P60" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q60" s="34" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="30" t="s">
-        <v>270</v>
-      </c>
-      <c r="B61" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="C61" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="D61" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="E61" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="F61" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="G61" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="H61" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="I61" s="31" t="s">
+      <c r="A61" s="33" t="s">
+        <v>273</v>
+      </c>
+      <c r="B61" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="C61" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="D61" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="E61" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="F61" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="G61" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="H61" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="I61" s="34" t="s">
         <v>179</v>
       </c>
-      <c r="J61" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="K61" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="L61" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="M61" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="N61" s="32" t="s">
-        <v>271</v>
-      </c>
-      <c r="O61" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="P61" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q61" s="31" t="s">
+      <c r="J61" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="K61" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="L61" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="M61" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="N61" s="35" t="s">
+        <v>274</v>
+      </c>
+      <c r="O61" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="P61" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q61" s="34" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="30" t="s">
-        <v>272</v>
-      </c>
-      <c r="B62" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="C62" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="D62" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="E62" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="F62" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="G62" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="H62" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="I62" s="31" t="s">
+      <c r="A62" s="33" t="s">
+        <v>275</v>
+      </c>
+      <c r="B62" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="C62" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="D62" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="E62" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="F62" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="G62" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="H62" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="I62" s="34" t="s">
         <v>184</v>
       </c>
-      <c r="J62" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="K62" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="L62" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="M62" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="N62" s="32" t="s">
-        <v>273</v>
-      </c>
-      <c r="O62" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="P62" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q62" s="31" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="63" s="37" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="35" t="s">
-        <v>274</v>
-      </c>
-      <c r="B63" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="C63" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="D63" s="36" t="s">
+      <c r="J62" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="K62" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="L62" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="M62" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="N62" s="35" t="s">
+        <v>276</v>
+      </c>
+      <c r="O62" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="P62" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q62" s="34" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="63" s="40" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="38" t="s">
+        <v>277</v>
+      </c>
+      <c r="B63" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="C63" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="D63" s="39" t="s">
         <v>144</v>
       </c>
-      <c r="E63" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="F63" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="G63" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="H63" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="I63" s="36" t="s">
+      <c r="E63" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="F63" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="G63" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="H63" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="I63" s="39" t="s">
         <v>190</v>
       </c>
-      <c r="J63" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="K63" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="L63" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="M63" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="N63" s="36" t="s">
-        <v>275</v>
-      </c>
-      <c r="O63" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="P63" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q63" s="36" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="64" s="37" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="35" t="s">
-        <v>276</v>
-      </c>
-      <c r="B64" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="C64" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="D64" s="36" t="s">
+      <c r="J63" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="K63" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="L63" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="M63" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="N63" s="39" t="s">
+        <v>278</v>
+      </c>
+      <c r="O63" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="P63" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q63" s="39" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="64" s="40" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="38" t="s">
+        <v>279</v>
+      </c>
+      <c r="B64" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="C64" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="D64" s="39" t="s">
         <v>149</v>
       </c>
-      <c r="E64" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="F64" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="G64" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="H64" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="I64" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="J64" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="K64" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="L64" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="M64" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="N64" s="36" t="s">
-        <v>277</v>
-      </c>
-      <c r="O64" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="P64" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q64" s="36" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="65" s="33" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="30" t="s">
-        <v>278</v>
-      </c>
-      <c r="B65" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="C65" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="D65" s="31" t="s">
+      <c r="E64" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="F64" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="G64" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="H64" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="I64" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="J64" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="K64" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="L64" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="M64" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="N64" s="39" t="s">
+        <v>280</v>
+      </c>
+      <c r="O64" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="P64" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q64" s="39" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="65" s="36" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="33" t="s">
+        <v>281</v>
+      </c>
+      <c r="B65" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="C65" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="D65" s="34" t="s">
         <v>154</v>
       </c>
-      <c r="E65" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="F65" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="G65" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="H65" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="I65" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="J65" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="K65" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="L65" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="M65" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="N65" s="32" t="s">
-        <v>279</v>
-      </c>
-      <c r="O65" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="P65" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q65" s="31" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="66" s="33" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="30" t="s">
-        <v>280</v>
-      </c>
-      <c r="B66" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="C66" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="D66" s="31" t="s">
+      <c r="E65" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="F65" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="G65" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="H65" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="I65" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="J65" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="K65" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="L65" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="M65" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="N65" s="35" t="s">
+        <v>282</v>
+      </c>
+      <c r="O65" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="P65" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q65" s="34" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="66" s="36" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="33" t="s">
+        <v>283</v>
+      </c>
+      <c r="B66" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="C66" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="D66" s="34" t="s">
         <v>160</v>
       </c>
-      <c r="E66" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="F66" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="G66" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="H66" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="I66" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="J66" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="K66" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="L66" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="M66" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="N66" s="32" t="s">
-        <v>281</v>
-      </c>
-      <c r="O66" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="P66" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q66" s="31" t="s">
+      <c r="E66" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="F66" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="G66" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="H66" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="I66" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="J66" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="K66" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="L66" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="M66" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="N66" s="35" t="s">
+        <v>284</v>
+      </c>
+      <c r="O66" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="P66" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q66" s="34" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="5" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="B67" s="6" t="s">
         <v>32</v>
@@ -5205,7 +5245,7 @@
         <v>32</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="E67" s="6" t="s">
         <v>32</v>
@@ -5235,7 +5275,7 @@
         <v>32</v>
       </c>
       <c r="N67" s="6" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="O67" s="6" t="s">
         <v>225</v>
@@ -5249,7 +5289,7 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="5" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="B68" s="6" t="s">
         <v>32</v>
@@ -5288,7 +5328,7 @@
         <v>32</v>
       </c>
       <c r="N68" s="6" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="O68" s="6" t="s">
         <v>232</v>
@@ -5302,10 +5342,10 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="5" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="C69" s="6" t="s">
         <v>32</v>
@@ -5341,7 +5381,7 @@
         <v>156</v>
       </c>
       <c r="N69" s="6" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="O69" s="6" t="s">
         <v>32</v>
@@ -5355,10 +5395,10 @@
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="5" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="C70" s="6" t="s">
         <v>32</v>
@@ -5394,7 +5434,7 @@
         <v>32</v>
       </c>
       <c r="N70" s="6" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="O70" s="6" t="s">
         <v>32</v>
@@ -5408,10 +5448,10 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="5" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="C71" s="6" t="s">
         <v>32</v>
@@ -5447,7 +5487,7 @@
         <v>32</v>
       </c>
       <c r="N71" s="6" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="O71" s="6" t="s">
         <v>239</v>
@@ -5461,10 +5501,10 @@
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="5" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="C72" s="6" t="s">
         <v>32</v>
@@ -5500,7 +5540,7 @@
         <v>32</v>
       </c>
       <c r="N72" s="6" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="O72" s="6" t="s">
         <v>158</v>
@@ -5514,10 +5554,10 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="5" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="C73" s="6" t="s">
         <v>32</v>
@@ -5553,7 +5593,7 @@
         <v>32</v>
       </c>
       <c r="N73" s="6" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="O73" s="6" t="s">
         <v>164</v>
@@ -5565,486 +5605,486 @@
         <v>32</v>
       </c>
     </row>
-    <row r="74" s="33" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="30" t="s">
-        <v>302</v>
-      </c>
-      <c r="B74" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="C74" s="31" t="s">
+    <row r="74" s="36" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="33" t="s">
+        <v>305</v>
+      </c>
+      <c r="B74" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="C74" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="D74" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="E74" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="F74" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="G74" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="H74" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="I74" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="J74" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="K74" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="L74" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="M74" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="N74" s="32" t="s">
-        <v>303</v>
-      </c>
-      <c r="O74" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="P74" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q74" s="31" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="75" s="33" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="30" t="s">
-        <v>304</v>
-      </c>
-      <c r="B75" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="C75" s="31" t="s">
+      <c r="D74" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="E74" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="F74" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="G74" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="H74" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="I74" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="J74" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="K74" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="L74" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="M74" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="N74" s="35" t="s">
+        <v>306</v>
+      </c>
+      <c r="O74" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="P74" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q74" s="34" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="75" s="36" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="33" t="s">
+        <v>307</v>
+      </c>
+      <c r="B75" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="C75" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="D75" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="E75" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="F75" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="G75" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="H75" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="I75" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="J75" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="K75" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="L75" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="M75" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="N75" s="32" t="s">
-        <v>305</v>
-      </c>
-      <c r="O75" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="P75" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q75" s="31" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="76" s="33" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="30" t="s">
-        <v>306</v>
-      </c>
-      <c r="B76" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="C76" s="31" t="s">
+      <c r="D75" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="E75" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="F75" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="G75" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="H75" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="I75" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="J75" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="K75" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="L75" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="M75" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="N75" s="35" t="s">
+        <v>308</v>
+      </c>
+      <c r="O75" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="P75" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q75" s="34" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="76" s="36" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="33" t="s">
+        <v>309</v>
+      </c>
+      <c r="B76" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="C76" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="D76" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="E76" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="F76" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="G76" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="H76" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="I76" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="J76" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="K76" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="L76" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="M76" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="N76" s="32" t="s">
-        <v>307</v>
-      </c>
-      <c r="O76" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="P76" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q76" s="31" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="77" s="33" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="30" t="s">
-        <v>308</v>
-      </c>
-      <c r="B77" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="C77" s="31" t="s">
+      <c r="D76" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="E76" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="F76" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="G76" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="H76" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="I76" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="J76" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="K76" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="L76" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="M76" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="N76" s="35" t="s">
+        <v>310</v>
+      </c>
+      <c r="O76" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="P76" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q76" s="34" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="77" s="36" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="33" t="s">
+        <v>311</v>
+      </c>
+      <c r="B77" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="C77" s="34" t="s">
         <v>117</v>
       </c>
-      <c r="D77" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="E77" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="F77" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="G77" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="H77" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="I77" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="J77" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="K77" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="L77" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="M77" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="N77" s="32" t="s">
-        <v>309</v>
-      </c>
-      <c r="O77" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="P77" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q77" s="31" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="78" s="33" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="30" t="s">
-        <v>310</v>
-      </c>
-      <c r="B78" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="C78" s="31" t="s">
+      <c r="D77" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="E77" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="F77" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="G77" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="H77" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="I77" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="J77" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="K77" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="L77" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="M77" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="N77" s="35" t="s">
+        <v>312</v>
+      </c>
+      <c r="O77" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="P77" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q77" s="34" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="78" s="36" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="33" t="s">
+        <v>313</v>
+      </c>
+      <c r="B78" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="C78" s="34" t="s">
         <v>89</v>
       </c>
-      <c r="D78" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="E78" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="F78" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="G78" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="H78" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="I78" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="J78" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="K78" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="L78" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="M78" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="N78" s="32" t="s">
-        <v>311</v>
-      </c>
-      <c r="O78" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="P78" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q78" s="31" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="79" s="33" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="30" t="s">
-        <v>312</v>
-      </c>
-      <c r="B79" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="C79" s="31" t="s">
+      <c r="D78" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="E78" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="F78" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="G78" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="H78" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="I78" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="J78" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="K78" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="L78" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="M78" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="N78" s="35" t="s">
+        <v>314</v>
+      </c>
+      <c r="O78" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="P78" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q78" s="34" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="79" s="36" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="33" t="s">
+        <v>315</v>
+      </c>
+      <c r="B79" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="C79" s="34" t="s">
         <v>123</v>
       </c>
-      <c r="D79" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="E79" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="F79" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="G79" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="H79" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="I79" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="J79" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="K79" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="L79" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="M79" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="N79" s="32" t="s">
-        <v>313</v>
-      </c>
-      <c r="O79" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="P79" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q79" s="31" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="80" s="33" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="30" t="s">
-        <v>314</v>
-      </c>
-      <c r="B80" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="C80" s="31" t="s">
+      <c r="D79" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="E79" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="F79" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="G79" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="H79" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="I79" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="J79" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="K79" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="L79" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="M79" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="N79" s="35" t="s">
+        <v>316</v>
+      </c>
+      <c r="O79" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="P79" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q79" s="34" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="80" s="36" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="33" t="s">
+        <v>317</v>
+      </c>
+      <c r="B80" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="C80" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="D80" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="E80" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="F80" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="G80" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="H80" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="I80" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="J80" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="K80" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="L80" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="M80" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="N80" s="32" t="s">
-        <v>315</v>
-      </c>
-      <c r="O80" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="P80" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q80" s="31" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="81" s="33" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="30" t="s">
-        <v>316</v>
-      </c>
-      <c r="B81" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="C81" s="31" t="s">
+      <c r="D80" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="E80" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="F80" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="G80" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="H80" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="I80" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="J80" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="K80" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="L80" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="M80" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="N80" s="35" t="s">
+        <v>318</v>
+      </c>
+      <c r="O80" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="P80" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q80" s="34" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="81" s="36" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="33" t="s">
+        <v>319</v>
+      </c>
+      <c r="B81" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="C81" s="34" t="s">
         <v>99</v>
       </c>
-      <c r="D81" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="E81" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="F81" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="G81" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="H81" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="I81" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="J81" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="K81" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="L81" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="M81" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="N81" s="32" t="s">
-        <v>317</v>
-      </c>
-      <c r="O81" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="P81" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q81" s="31" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="82" s="33" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="30" t="s">
-        <v>318</v>
-      </c>
-      <c r="B82" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="C82" s="31" t="s">
+      <c r="D81" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="E81" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="F81" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="G81" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="H81" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="I81" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="J81" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="K81" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="L81" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="M81" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="N81" s="35" t="s">
+        <v>320</v>
+      </c>
+      <c r="O81" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="P81" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q81" s="34" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="82" s="36" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="33" t="s">
+        <v>321</v>
+      </c>
+      <c r="B82" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="C82" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="D82" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="E82" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="F82" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="G82" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="H82" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="I82" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="J82" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="K82" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="L82" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="M82" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="N82" s="32" t="s">
-        <v>319</v>
-      </c>
-      <c r="O82" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="P82" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q82" s="31" t="s">
+      <c r="D82" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="E82" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="F82" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="G82" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="H82" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="I82" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="J82" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="K82" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="L82" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="M82" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="N82" s="35" t="s">
+        <v>322</v>
+      </c>
+      <c r="O82" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="P82" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q82" s="34" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="5" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="B83" s="6" t="s">
         <v>32</v>
@@ -6083,7 +6123,7 @@
         <v>32</v>
       </c>
       <c r="N83" s="6" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="O83" s="6" t="s">
         <v>32</v>
@@ -6097,7 +6137,7 @@
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="5" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="B84" s="6" t="s">
         <v>32</v>
@@ -6136,7 +6176,7 @@
         <v>32</v>
       </c>
       <c r="N84" s="6" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="O84" s="6" t="s">
         <v>32</v>
@@ -6150,7 +6190,7 @@
     </row>
     <row r="85" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="5" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="B85" s="6" t="s">
         <v>32</v>
@@ -6189,7 +6229,7 @@
         <v>32</v>
       </c>
       <c r="N85" s="6" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="O85" s="6" t="s">
         <v>32</v>
@@ -6203,7 +6243,7 @@
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="5" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="B86" s="6" t="s">
         <v>32</v>
@@ -6242,7 +6282,7 @@
         <v>32</v>
       </c>
       <c r="N86" s="6" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="O86" s="6" t="s">
         <v>32</v>
@@ -6256,7 +6296,7 @@
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="5" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="B87" s="6" t="s">
         <v>32</v>
@@ -6295,7 +6335,7 @@
         <v>32</v>
       </c>
       <c r="N87" s="6" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="O87" s="6" t="s">
         <v>32</v>
@@ -6309,7 +6349,7 @@
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="5" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="B88" s="6" t="s">
         <v>32</v>
@@ -6348,7 +6388,7 @@
         <v>32</v>
       </c>
       <c r="N88" s="6" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="O88" s="6" t="s">
         <v>32</v>
@@ -6362,7 +6402,7 @@
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="5" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="B89" s="6" t="s">
         <v>32</v>
@@ -6399,7 +6439,7 @@
         <v>32</v>
       </c>
       <c r="N89" s="6" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="O89" s="6" t="s">
         <v>32</v>
@@ -6413,7 +6453,7 @@
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="5" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="B90" s="6" t="s">
         <v>32</v>
@@ -6450,7 +6490,7 @@
         <v>32</v>
       </c>
       <c r="N90" s="6" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="O90" s="6" t="s">
         <v>32</v>
@@ -6464,7 +6504,7 @@
     </row>
     <row r="91" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="5" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="B91" s="6" t="s">
         <v>32</v>
@@ -6503,7 +6543,7 @@
         <v>32</v>
       </c>
       <c r="N91" s="7" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="O91" s="6" t="s">
         <v>32</v>
@@ -6517,7 +6557,7 @@
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="5" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="B92" s="6" t="s">
         <v>32</v>
@@ -6556,7 +6596,7 @@
         <v>32</v>
       </c>
       <c r="N92" s="6" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="O92" s="6" t="s">
         <v>32</v>
@@ -6570,7 +6610,7 @@
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="5" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="B93" s="6" t="s">
         <v>32</v>
@@ -6609,7 +6649,7 @@
         <v>32</v>
       </c>
       <c r="N93" s="6" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="O93" s="6" t="s">
         <v>32</v>
@@ -6623,7 +6663,7 @@
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="5" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="B94" s="6" t="s">
         <v>32</v>
@@ -6665,7 +6705,7 @@
         <v>32</v>
       </c>
       <c r="O94" s="6" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="P94" s="6" t="s">
         <v>32</v>
@@ -6676,7 +6716,7 @@
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="5" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="B95" s="6" t="s">
         <v>32</v>
@@ -6715,7 +6755,7 @@
         <v>32</v>
       </c>
       <c r="N95" s="6" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="O95" s="6" t="s">
         <v>32</v>
@@ -6729,7 +6769,7 @@
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="5" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="B96" s="6" t="s">
         <v>32</v>
@@ -6768,7 +6808,7 @@
         <v>32</v>
       </c>
       <c r="N96" s="6" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="O96" s="6" t="s">
         <v>32</v>
@@ -6782,7 +6822,7 @@
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="5" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="B97" s="6" t="s">
         <v>32</v>
@@ -6821,7 +6861,7 @@
         <v>32</v>
       </c>
       <c r="N97" s="6" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="O97" s="6" t="s">
         <v>32</v>
@@ -6835,7 +6875,7 @@
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="5" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="B98" s="6" t="s">
         <v>32</v>
@@ -6874,7 +6914,7 @@
         <v>32</v>
       </c>
       <c r="N98" s="6" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="O98" s="6" t="s">
         <v>32</v>
@@ -6888,7 +6928,7 @@
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="5" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="B99" s="6" t="s">
         <v>32</v>
@@ -6927,7 +6967,7 @@
         <v>32</v>
       </c>
       <c r="N99" s="6" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="O99" s="6" t="s">
         <v>32</v>
@@ -6941,7 +6981,7 @@
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="5" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="B100" s="6" t="s">
         <v>32</v>
@@ -6980,7 +7020,7 @@
         <v>32</v>
       </c>
       <c r="N100" s="6" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="O100" s="6" t="s">
         <v>32</v>
@@ -6994,7 +7034,7 @@
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="5" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="B101" s="6" t="s">
         <v>32</v>
@@ -7033,7 +7073,7 @@
         <v>32</v>
       </c>
       <c r="N101" s="6" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="O101" s="6" t="s">
         <v>32</v>
@@ -7047,7 +7087,7 @@
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="5" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="B102" s="6" t="s">
         <v>32</v>
@@ -7086,7 +7126,7 @@
         <v>32</v>
       </c>
       <c r="N102" s="6" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="O102" s="6" t="s">
         <v>32</v>
@@ -7100,7 +7140,7 @@
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="5" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
       <c r="B103" s="6" t="s">
         <v>32</v>
@@ -7139,7 +7179,7 @@
         <v>32</v>
       </c>
       <c r="N103" s="6" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="O103" s="6" t="s">
         <v>32</v>
@@ -7153,7 +7193,7 @@
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="5" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B104" s="6" t="s">
         <v>32</v>
@@ -7192,7 +7232,7 @@
         <v>32</v>
       </c>
       <c r="N104" s="6" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="O104" s="6" t="s">
         <v>32</v>
@@ -7206,7 +7246,7 @@
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="5" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="B105" s="6" t="s">
         <v>32</v>
@@ -7245,7 +7285,7 @@
         <v>32</v>
       </c>
       <c r="N105" s="6" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="O105" s="6" t="s">
         <v>32</v>
@@ -7259,7 +7299,7 @@
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="5" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
       <c r="B106" s="6" t="s">
         <v>32</v>
@@ -7298,7 +7338,7 @@
         <v>32</v>
       </c>
       <c r="N106" s="6" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="O106" s="6" t="s">
         <v>32</v>
@@ -7312,7 +7352,7 @@
     </row>
     <row r="107" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="5" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="B107" s="6" t="s">
         <v>32</v>
@@ -7339,7 +7379,7 @@
         <v>32</v>
       </c>
       <c r="J107" s="7" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="K107" s="6" t="s">
         <v>32</v>
@@ -7365,7 +7405,7 @@
     </row>
     <row r="108" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="5" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="B108" s="6" t="s">
         <v>32</v>
@@ -7404,7 +7444,7 @@
         <v>32</v>
       </c>
       <c r="N108" s="7" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="O108" s="6" t="s">
         <v>32</v>
@@ -7418,7 +7458,7 @@
     </row>
     <row r="109" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="5" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="B109" s="6" t="s">
         <v>32</v>
@@ -7457,7 +7497,7 @@
         <v>32</v>
       </c>
       <c r="N109" s="7" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="O109" s="6" t="s">
         <v>32</v>
@@ -7471,7 +7511,7 @@
     </row>
     <row r="110" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="5" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="B110" s="6" t="s">
         <v>32</v>
@@ -7507,10 +7547,10 @@
         <v>32</v>
       </c>
       <c r="M110" s="7" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="N110" s="7" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
       <c r="O110" s="6" t="s">
         <v>32</v>
@@ -7524,7 +7564,7 @@
     </row>
     <row r="111" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="5" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="B111" s="6" t="s">
         <v>32</v>
@@ -7551,7 +7591,7 @@
         <v>32</v>
       </c>
       <c r="J111" s="7" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="K111" s="6" t="s">
         <v>32</v>
@@ -7563,7 +7603,7 @@
         <v>32</v>
       </c>
       <c r="N111" s="6" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="O111" s="6" t="s">
         <v>32</v>
@@ -7577,7 +7617,7 @@
     </row>
     <row r="112" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="5" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="B112" s="6" t="s">
         <v>32</v>
@@ -7604,7 +7644,7 @@
         <v>32</v>
       </c>
       <c r="J112" s="6" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="K112" s="6" t="s">
         <v>32</v>
@@ -7613,10 +7653,10 @@
         <v>32</v>
       </c>
       <c r="M112" s="7" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
       <c r="N112" s="6" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="O112" s="6" t="s">
         <v>32</v>
@@ -7630,7 +7670,7 @@
     </row>
     <row r="113" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="5" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="B113" s="6" t="s">
         <v>32</v>
@@ -7669,7 +7709,7 @@
         <v>186</v>
       </c>
       <c r="N113" s="6" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
       <c r="O113" s="6" t="s">
         <v>32</v>
@@ -7683,7 +7723,7 @@
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="5" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="B114" s="6" t="s">
         <v>32</v>
@@ -7710,7 +7750,7 @@
         <v>32</v>
       </c>
       <c r="J114" s="6" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="K114" s="6" t="s">
         <v>32</v>
@@ -7725,7 +7765,7 @@
         <v>32</v>
       </c>
       <c r="O114" s="6" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="P114" s="6" t="s">
         <v>32</v>
@@ -7736,7 +7776,7 @@
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="5" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
       <c r="B115" s="6" t="s">
         <v>32</v>
@@ -7789,7 +7829,7 @@
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="5" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
       <c r="B116" s="6" t="s">
         <v>32</v>
@@ -7842,7 +7882,7 @@
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="5" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="B117" s="6" t="s">
         <v>32</v>
@@ -7895,7 +7935,7 @@
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="5" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
       <c r="B118" s="6" t="s">
         <v>32</v>
@@ -7948,7 +7988,7 @@
     </row>
     <row r="119" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="5" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
       <c r="B119" s="6" t="s">
         <v>32</v>
@@ -8001,7 +8041,7 @@
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="5" t="s">
-        <v>392</v>
+        <v>395</v>
       </c>
       <c r="B120" s="6" t="s">
         <v>32</v>
@@ -8054,7 +8094,7 @@
     </row>
     <row r="121" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="5" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="B121" s="6" t="s">
         <v>32</v>
@@ -8107,7 +8147,7 @@
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="5" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
       <c r="B122" s="6" t="s">
         <v>32</v>
@@ -8160,7 +8200,7 @@
     </row>
     <row r="123" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="5" t="s">
-        <v>395</v>
+        <v>398</v>
       </c>
       <c r="B123" s="6" t="s">
         <v>32</v>
@@ -8213,7 +8253,7 @@
     </row>
     <row r="124" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="5" t="s">
-        <v>396</v>
+        <v>399</v>
       </c>
       <c r="B124" s="6" t="s">
         <v>32</v>
@@ -8266,7 +8306,7 @@
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="5" t="s">
-        <v>397</v>
+        <v>400</v>
       </c>
       <c r="B125" s="6" t="s">
         <v>32</v>
@@ -8275,7 +8315,7 @@
         <v>32</v>
       </c>
       <c r="D125" s="6" t="s">
-        <v>398</v>
+        <v>401</v>
       </c>
       <c r="E125" s="6" t="s">
         <v>32</v>
@@ -8319,7 +8359,7 @@
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="5" t="s">
-        <v>399</v>
+        <v>402</v>
       </c>
       <c r="B126" s="6" t="s">
         <v>32</v>
@@ -8328,7 +8368,7 @@
         <v>32</v>
       </c>
       <c r="D126" s="6" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="E126" s="6" t="s">
         <v>32</v>
@@ -8372,7 +8412,7 @@
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="5" t="s">
-        <v>401</v>
+        <v>404</v>
       </c>
       <c r="B127" s="6" t="s">
         <v>32</v>
@@ -8381,7 +8421,7 @@
         <v>32</v>
       </c>
       <c r="D127" s="6" t="s">
-        <v>402</v>
+        <v>405</v>
       </c>
       <c r="E127" s="6" t="s">
         <v>32</v>
@@ -8425,7 +8465,7 @@
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="5" t="s">
-        <v>403</v>
+        <v>406</v>
       </c>
       <c r="B128" s="6" t="s">
         <v>32</v>
@@ -8464,7 +8504,7 @@
       <c r="N128" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="O128" s="29" t="s">
+      <c r="O128" s="41" t="s">
         <v>32</v>
       </c>
       <c r="P128" s="6" t="s">
@@ -8476,7 +8516,7 @@
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="5" t="s">
-        <v>404</v>
+        <v>407</v>
       </c>
       <c r="B129" s="6" t="s">
         <v>32</v>
@@ -8529,7 +8569,7 @@
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="5" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="B130" s="6" t="s">
         <v>32</v>
@@ -8571,7 +8611,7 @@
         <v>32</v>
       </c>
       <c r="O130" s="6" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="P130" s="6" t="s">
         <v>32</v>
@@ -8582,7 +8622,7 @@
     </row>
     <row r="131" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="5" t="s">
-        <v>406</v>
+        <v>409</v>
       </c>
       <c r="B131" s="6" t="s">
         <v>32</v>
@@ -8591,7 +8631,7 @@
         <v>32</v>
       </c>
       <c r="D131" s="6" t="s">
-        <v>407</v>
+        <v>410</v>
       </c>
       <c r="E131" s="6" t="s">
         <v>32</v>
@@ -8624,7 +8664,7 @@
         <v>32</v>
       </c>
       <c r="O131" s="6" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="P131" s="6" t="s">
         <v>32</v>
@@ -8635,7 +8675,7 @@
     </row>
     <row r="132" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="5" t="s">
-        <v>408</v>
+        <v>411</v>
       </c>
       <c r="B132" s="6" t="s">
         <v>32</v>
@@ -8688,7 +8728,7 @@
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="5" t="s">
-        <v>409</v>
+        <v>412</v>
       </c>
       <c r="B133" s="6" t="s">
         <v>32</v>
@@ -8741,7 +8781,7 @@
     </row>
     <row r="134" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="5" t="s">
-        <v>410</v>
+        <v>413</v>
       </c>
       <c r="B134" s="6" t="s">
         <v>32</v>
@@ -8794,7 +8834,7 @@
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="5" t="s">
-        <v>411</v>
+        <v>414</v>
       </c>
       <c r="B135" s="6" t="s">
         <v>32</v>
@@ -8847,7 +8887,7 @@
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="5" t="s">
-        <v>412</v>
+        <v>415</v>
       </c>
       <c r="B136" s="6" t="s">
         <v>32</v>
@@ -8900,7 +8940,7 @@
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="5" t="s">
-        <v>413</v>
+        <v>416</v>
       </c>
       <c r="B137" s="6" t="s">
         <v>32</v>
@@ -8953,7 +8993,7 @@
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="5" t="s">
-        <v>414</v>
+        <v>417</v>
       </c>
       <c r="B138" s="6" t="s">
         <v>32</v>
@@ -9006,7 +9046,7 @@
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="5" t="s">
-        <v>415</v>
+        <v>418</v>
       </c>
       <c r="B139" s="6" t="s">
         <v>32</v>
@@ -9059,7 +9099,7 @@
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="5" t="s">
-        <v>416</v>
+        <v>419</v>
       </c>
       <c r="B140" s="6" t="s">
         <v>32</v>
@@ -9112,7 +9152,7 @@
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="5" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="B141" s="6" t="s">
         <v>32</v>
@@ -9165,7 +9205,7 @@
     </row>
     <row r="142" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="5" t="s">
-        <v>418</v>
+        <v>421</v>
       </c>
       <c r="B142" s="6" t="s">
         <v>32</v>
@@ -9224,7 +9264,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CSeite &amp;P</oddFooter>

</xml_diff>

<commit_message>
stm32f4_function_mappings.xml: fix ethernet pinout
</commit_message>
<xml_diff>
--- a/platform/embedded/stm32f407/stm32f4_function_mappings.xlsx
+++ b/platform/embedded/stm32f407/stm32f4_function_mappings.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2405" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2404" uniqueCount="422">
   <si>
     <t xml:space="preserve">Port</t>
   </si>
@@ -692,30 +692,30 @@
 NXT</t>
   </si>
   <si>
-    <t xml:space="preserve">PC4</t>
-  </si>
-  <si>
     <t xml:space="preserve">ETH
 _MII_TX_CLK</t>
   </si>
   <si>
+    <t xml:space="preserve">PC4</t>
+  </si>
+  <si>
     <t xml:space="preserve">PC5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PC6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TIM8_CH1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I2S2_MCK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">USART6_TX</t>
   </si>
   <si>
     <t xml:space="preserve">ETH_MII_RXD1
 ETH_RMII_RXD1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PC6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TIM8_CH1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I2S2_MCK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USART6_TX</t>
   </si>
   <si>
     <t xml:space="preserve">SDIO_D6</t>
@@ -1477,7 +1477,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="51">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1518,12 +1518,16 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1570,8 +1574,16 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -1579,6 +1591,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1596,10 +1612,6 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1750,11 +1762,11 @@
   <dimension ref="A1:R142"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B19" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="C18" activeCellId="0" sqref="C18"/>
+      <selection pane="bottomLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
+      <selection pane="bottomRight" activeCell="M40" activeCellId="0" sqref="M40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1929,7 +1941,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" s="11" customFormat="true" ht="57.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" s="11" customFormat="true" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
         <v>39</v>
       </c>
@@ -2019,7 +2031,7 @@
       <c r="L5" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="M5" s="9" t="s">
+      <c r="M5" s="12" t="s">
         <v>50</v>
       </c>
       <c r="N5" s="9" t="s">
@@ -2247,7 +2259,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" s="11" customFormat="true" ht="37.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" s="11" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="8" t="s">
         <v>76</v>
       </c>
@@ -2353,215 +2365,215 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" s="15" customFormat="true" ht="25.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="12" t="s">
+    <row r="12" s="16" customFormat="true" ht="25.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="B12" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" s="13" t="s">
+      <c r="B12" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="D12" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="E12" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="F12" s="14" t="s">
+      <c r="D12" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="G12" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="H12" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="I12" s="13" t="s">
+      <c r="G12" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="H12" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="I12" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="J12" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="K12" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="L12" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="M12" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="N12" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="O12" s="13" t="s">
+      <c r="J12" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="K12" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="L12" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="M12" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="N12" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="O12" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="P12" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q12" s="13" t="s">
+      <c r="P12" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q12" s="14" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="B13" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="13" t="s">
+      <c r="B13" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="D13" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="E13" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="F13" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="G13" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="H13" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="I13" s="13" t="s">
+      <c r="D13" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="H13" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="I13" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="J13" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="K13" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="L13" s="16" t="s">
+      <c r="J13" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="K13" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="L13" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="M13" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="N13" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="O13" s="13" t="s">
+      <c r="M13" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="N13" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="O13" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="P13" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q13" s="13" t="s">
+      <c r="P13" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q13" s="14" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="B14" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="13" t="s">
+      <c r="B14" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="D14" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="F14" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="G14" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="H14" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="I14" s="13" t="s">
+      <c r="D14" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="G14" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="H14" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="I14" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="J14" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="K14" s="13" t="s">
+      <c r="J14" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="K14" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="L14" s="16" t="s">
+      <c r="L14" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="M14" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="N14" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="O14" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="P14" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q14" s="13" t="s">
+      <c r="M14" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="N14" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="O14" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="P14" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q14" s="14" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="B15" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" s="13" t="s">
+      <c r="B15" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="D15" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="E15" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="F15" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="G15" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="H15" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="I15" s="13" t="s">
+      <c r="D15" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="G15" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="H15" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="I15" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="J15" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="K15" s="13" t="s">
+      <c r="J15" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="K15" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="L15" s="16" t="s">
+      <c r="L15" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="M15" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="N15" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="O15" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="P15" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q15" s="13" t="s">
+      <c r="M15" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="N15" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="O15" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="P15" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q15" s="14" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2830,311 +2842,311 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" s="19" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="17" t="s">
+    <row r="21" s="20" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="B21" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="C21" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="D21" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="E21" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="F21" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="G21" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="H21" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="I21" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="J21" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="K21" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="L21" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="M21" s="18"/>
-      <c r="N21" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="O21" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="P21" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q21" s="18" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" s="23" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="20" t="s">
+      <c r="B21" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="F21" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="G21" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="H21" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="I21" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="J21" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="K21" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="L21" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="M21" s="19"/>
+      <c r="N21" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="O21" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="P21" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q21" s="19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" s="25" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="21" t="s">
         <v>129</v>
       </c>
-      <c r="B22" s="21" t="s">
+      <c r="B22" s="22" t="s">
         <v>130</v>
       </c>
-      <c r="C22" s="22" t="s">
+      <c r="C22" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="D22" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="E22" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="F22" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="G22" s="22" t="s">
+      <c r="D22" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="E22" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="F22" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="G22" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="H22" s="21" t="s">
+      <c r="H22" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="I22" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="J22" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="K22" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="L22" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="M22" s="22"/>
-      <c r="N22" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="O22" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="P22" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q22" s="22" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="23" s="23" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="20" t="s">
+      <c r="I22" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="J22" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="K22" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="L22" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="M22" s="23"/>
+      <c r="N22" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="O22" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="P22" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q22" s="23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" s="25" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="B23" s="22" t="s">
+      <c r="B23" s="23" t="s">
         <v>133</v>
       </c>
-      <c r="C23" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="D23" s="22" t="s">
+      <c r="C23" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="E23" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="F23" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="G23" s="22" t="s">
+      <c r="E23" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="F23" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="G23" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="H23" s="22" t="s">
+      <c r="H23" s="26" t="s">
         <v>134</v>
       </c>
-      <c r="I23" s="22" t="s">
+      <c r="I23" s="23" t="s">
         <v>135</v>
       </c>
-      <c r="J23" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="K23" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="L23" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="M23" s="22"/>
-      <c r="N23" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="O23" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="P23" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q23" s="22" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="24" s="23" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="20" t="s">
+      <c r="J23" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="K23" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="L23" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="M23" s="23"/>
+      <c r="N23" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="O23" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="P23" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q23" s="23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" s="25" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="B24" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="C24" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="D24" s="22" t="s">
+      <c r="B24" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="D24" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="E24" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="F24" s="21" t="s">
+      <c r="E24" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="F24" s="22" t="s">
         <v>137</v>
       </c>
-      <c r="G24" s="22" t="s">
+      <c r="G24" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="H24" s="21" t="s">
+      <c r="H24" s="24" t="s">
         <v>138</v>
       </c>
-      <c r="I24" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="J24" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="K24" s="22" t="s">
+      <c r="I24" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="J24" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="K24" s="23" t="s">
         <v>139</v>
       </c>
-      <c r="L24" s="21" t="s">
+      <c r="L24" s="22" t="s">
         <v>140</v>
       </c>
-      <c r="M24" s="22" t="s">
+      <c r="M24" s="23" t="s">
         <v>141</v>
       </c>
-      <c r="N24" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="O24" s="22" t="s">
+      <c r="N24" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="O24" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="P24" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q24" s="22" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="25" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="12" t="s">
+      <c r="P24" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q24" s="23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="B25" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="C25" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="D25" s="13" t="s">
+      <c r="B25" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="E25" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="F25" s="13" t="s">
+      <c r="E25" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F25" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="G25" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="H25" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="I25" s="16" t="s">
+      <c r="G25" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="H25" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="I25" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="J25" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="K25" s="13" t="s">
+      <c r="J25" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="K25" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="L25" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="M25" s="13"/>
-      <c r="N25" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="O25" s="13" t="s">
+      <c r="L25" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="M25" s="14"/>
+      <c r="N25" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="O25" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="P25" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q25" s="13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="26" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="12" t="s">
+      <c r="P25" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q25" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="B26" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="C26" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="D26" s="13" t="s">
+      <c r="B26" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D26" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="E26" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="F26" s="13" t="s">
+      <c r="E26" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F26" s="14" t="s">
         <v>150</v>
       </c>
-      <c r="G26" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="H26" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="I26" s="16" t="s">
+      <c r="G26" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="H26" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="I26" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="J26" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="K26" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="L26" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="M26" s="13"/>
-      <c r="N26" s="13" t="s">
+      <c r="J26" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="K26" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="L26" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="M26" s="14"/>
+      <c r="N26" s="14" t="s">
         <v>151</v>
       </c>
-      <c r="O26" s="15" t="s">
+      <c r="O26" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="P26" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q26" s="13" t="s">
+      <c r="P26" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q26" s="14" t="s">
         <v>32</v>
       </c>
     </row>
@@ -3242,56 +3254,56 @@
         <v>32</v>
       </c>
     </row>
-    <row r="29" s="19" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="17" t="s">
+    <row r="29" s="20" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="18" t="s">
         <v>165</v>
       </c>
-      <c r="B29" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="C29" s="18" t="s">
+      <c r="B29" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="D29" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="E29" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="F29" s="18" t="s">
+      <c r="D29" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="E29" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="F29" s="19" t="s">
         <v>166</v>
       </c>
-      <c r="G29" s="24" t="s">
+      <c r="G29" s="27" t="s">
         <v>167</v>
       </c>
-      <c r="H29" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="I29" s="18" t="s">
+      <c r="H29" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="I29" s="19" t="s">
         <v>168</v>
       </c>
-      <c r="J29" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="K29" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="L29" s="25" t="s">
+      <c r="J29" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="K29" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="L29" s="28" t="s">
         <v>169</v>
       </c>
-      <c r="M29" s="18" t="s">
+      <c r="M29" s="19" t="s">
         <v>170</v>
       </c>
-      <c r="N29" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="O29" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="P29" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q29" s="18" t="s">
+      <c r="N29" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="O29" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="P29" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q29" s="19" t="s">
         <v>32</v>
       </c>
     </row>
@@ -3329,7 +3341,7 @@
       <c r="K30" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="L30" s="10" t="s">
+      <c r="L30" s="29" t="s">
         <v>174</v>
       </c>
       <c r="M30" s="10" t="s">
@@ -3364,10 +3376,10 @@
       <c r="E31" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="F31" s="10" t="s">
+      <c r="F31" s="29" t="s">
         <v>177</v>
       </c>
-      <c r="G31" s="10" t="s">
+      <c r="G31" s="29" t="s">
         <v>178</v>
       </c>
       <c r="H31" s="9" t="s">
@@ -3382,7 +3394,7 @@
       <c r="K31" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="L31" s="10" t="s">
+      <c r="L31" s="29" t="s">
         <v>180</v>
       </c>
       <c r="M31" s="10" t="s">
@@ -3420,7 +3432,7 @@
       <c r="F32" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="G32" s="10" t="s">
+      <c r="G32" s="29" t="s">
         <v>167</v>
       </c>
       <c r="H32" s="9" t="s">
@@ -3435,7 +3447,7 @@
       <c r="K32" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="L32" s="10" t="s">
+      <c r="L32" s="29" t="s">
         <v>185</v>
       </c>
       <c r="M32" s="10" t="s">
@@ -3650,7 +3662,7 @@
       <c r="L36" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="M36" s="9" t="s">
+      <c r="M36" s="12" t="s">
         <v>201</v>
       </c>
       <c r="N36" s="9" t="s">
@@ -3666,56 +3678,56 @@
         <v>32</v>
       </c>
     </row>
-    <row r="37" s="19" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="17" t="s">
+    <row r="37" s="20" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="18" t="s">
         <v>202</v>
       </c>
-      <c r="B37" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="C37" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="D37" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="E37" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="F37" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="G37" s="26" t="s">
+      <c r="B37" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C37" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D37" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="E37" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="F37" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="G37" s="30" t="s">
         <v>188</v>
       </c>
-      <c r="H37" s="18" t="s">
+      <c r="H37" s="19" t="s">
         <v>189</v>
       </c>
-      <c r="I37" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="J37" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="K37" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="L37" s="25" t="s">
+      <c r="I37" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="J37" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="K37" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="L37" s="28" t="s">
         <v>203</v>
       </c>
-      <c r="M37" s="18" t="s">
+      <c r="M37" s="19" t="s">
         <v>204</v>
       </c>
-      <c r="N37" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="O37" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="P37" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q37" s="18" t="s">
+      <c r="N37" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="O37" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="P37" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q37" s="19" t="s">
         <v>32</v>
       </c>
     </row>
@@ -3756,8 +3768,8 @@
       <c r="L38" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="M38" s="6" t="s">
-        <v>204</v>
+      <c r="M38" s="7" t="s">
+        <v>207</v>
       </c>
       <c r="N38" s="6" t="s">
         <v>32</v>
@@ -3774,7 +3786,7 @@
     </row>
     <row r="39" s="11" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="8" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B39" s="9" t="s">
         <v>32</v>
@@ -3810,7 +3822,7 @@
         <v>32</v>
       </c>
       <c r="M39" s="10" t="s">
-        <v>208</v>
+        <v>181</v>
       </c>
       <c r="N39" s="9" t="s">
         <v>32</v>
@@ -3863,7 +3875,7 @@
         <v>32</v>
       </c>
       <c r="M40" s="10" t="s">
-        <v>181</v>
+        <v>210</v>
       </c>
       <c r="N40" s="9" t="s">
         <v>32</v>
@@ -3878,701 +3890,699 @@
         <v>32</v>
       </c>
     </row>
-    <row r="41" s="31" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="27" t="s">
-        <v>210</v>
-      </c>
-      <c r="B41" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="C41" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="D41" s="28" t="s">
+    <row r="41" s="34" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="31" t="s">
         <v>211</v>
       </c>
-      <c r="E41" s="28" t="s">
-        <v>211</v>
-      </c>
-      <c r="F41" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="G41" s="28" t="s">
+      <c r="B41" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="C41" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="D41" s="32" t="s">
         <v>212</v>
       </c>
-      <c r="H41" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="I41" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="J41" s="29" t="s">
+      <c r="E41" s="32" t="s">
+        <v>212</v>
+      </c>
+      <c r="F41" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="G41" s="32" t="s">
         <v>213</v>
       </c>
-      <c r="K41" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="L41" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="M41" s="30" t="s">
+      <c r="H41" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="I41" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="J41" s="33" t="s">
         <v>214</v>
       </c>
-      <c r="N41" s="28" t="s">
+      <c r="K41" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="L41" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="M41" s="32"/>
+      <c r="N41" s="32" t="s">
         <v>215</v>
       </c>
-      <c r="O41" s="28" t="s">
+      <c r="O41" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="P41" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q41" s="28" t="s">
+      <c r="P41" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q41" s="32" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="27" t="s">
+      <c r="A42" s="31" t="s">
         <v>216</v>
       </c>
-      <c r="B42" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="C42" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="D42" s="28" t="s">
+      <c r="B42" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="C42" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="D42" s="32" t="s">
         <v>217</v>
       </c>
-      <c r="E42" s="28" t="s">
+      <c r="E42" s="32" t="s">
         <v>217</v>
       </c>
-      <c r="F42" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="G42" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="H42" s="28" t="s">
+      <c r="F42" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="G42" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="H42" s="32" t="s">
         <v>218</v>
       </c>
-      <c r="I42" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="J42" s="29" t="s">
+      <c r="I42" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="J42" s="33" t="s">
         <v>219</v>
       </c>
-      <c r="K42" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="L42" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="M42" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="N42" s="28" t="s">
+      <c r="K42" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="L42" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="M42" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="N42" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="O42" s="28" t="s">
+      <c r="O42" s="32" t="s">
         <v>97</v>
       </c>
-      <c r="P42" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q42" s="28" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="43" s="35" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="32" t="s">
+      <c r="P42" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q42" s="32" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="43" s="38" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="35" t="s">
         <v>221</v>
       </c>
-      <c r="B43" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="C43" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="D43" s="33" t="s">
+      <c r="B43" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="C43" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="D43" s="36" t="s">
         <v>222</v>
       </c>
-      <c r="E43" s="33" t="s">
+      <c r="E43" s="36" t="s">
         <v>222</v>
       </c>
-      <c r="F43" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="G43" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="H43" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="I43" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="J43" s="33" t="s">
+      <c r="F43" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="G43" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="H43" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="I43" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="J43" s="36" t="s">
         <v>223</v>
       </c>
-      <c r="K43" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="L43" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="M43" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="N43" s="34" t="s">
+      <c r="K43" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="L43" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="M43" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="N43" s="37" t="s">
         <v>224</v>
       </c>
-      <c r="O43" s="33" t="s">
+      <c r="O43" s="36" t="s">
         <v>225</v>
       </c>
-      <c r="P43" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q43" s="33" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="44" s="35" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="32" t="s">
+      <c r="P43" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q43" s="36" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="44" s="38" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="35" t="s">
         <v>226</v>
       </c>
-      <c r="B44" s="33" t="s">
+      <c r="B44" s="36" t="s">
         <v>227</v>
       </c>
-      <c r="C44" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="D44" s="33" t="s">
+      <c r="C44" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="D44" s="36" t="s">
         <v>228</v>
       </c>
-      <c r="E44" s="33" t="s">
+      <c r="E44" s="36" t="s">
         <v>228</v>
       </c>
-      <c r="F44" s="33" t="s">
+      <c r="F44" s="36" t="s">
         <v>229</v>
       </c>
-      <c r="G44" s="33" t="s">
+      <c r="G44" s="36" t="s">
         <v>230</v>
       </c>
-      <c r="H44" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="I44" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="J44" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="K44" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="L44" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="M44" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="N44" s="34" t="s">
+      <c r="H44" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="I44" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="J44" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="K44" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="L44" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="M44" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="N44" s="37" t="s">
         <v>231</v>
       </c>
-      <c r="O44" s="33" t="s">
+      <c r="O44" s="36" t="s">
         <v>232</v>
       </c>
-      <c r="P44" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q44" s="33" t="s">
+      <c r="P44" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q44" s="36" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="32" t="s">
+      <c r="A45" s="35" t="s">
         <v>233</v>
       </c>
-      <c r="B45" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="C45" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="D45" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="E45" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="F45" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="G45" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="H45" s="36" t="s">
+      <c r="B45" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="C45" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="D45" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="E45" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="F45" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="G45" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="H45" s="39" t="s">
         <v>234</v>
       </c>
-      <c r="I45" s="33" t="s">
+      <c r="I45" s="36" t="s">
         <v>168</v>
       </c>
-      <c r="J45" s="33" t="s">
+      <c r="J45" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="K45" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="L45" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="M45" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="N45" s="34" t="s">
+      <c r="K45" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="L45" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="M45" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="N45" s="37" t="s">
         <v>235</v>
       </c>
-      <c r="O45" s="33" t="s">
+      <c r="O45" s="36" t="s">
         <v>236</v>
       </c>
-      <c r="P45" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q45" s="33" t="s">
+      <c r="P45" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q45" s="36" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="32" t="s">
+      <c r="A46" s="35" t="s">
         <v>237</v>
       </c>
-      <c r="B46" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="C46" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="D46" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="E46" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="F46" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="G46" s="33" t="s">
+      <c r="B46" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="C46" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="D46" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="E46" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="F46" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="G46" s="36" t="s">
         <v>135</v>
       </c>
-      <c r="H46" s="34" t="s">
+      <c r="H46" s="37" t="s">
         <v>134</v>
       </c>
-      <c r="I46" s="33" t="s">
+      <c r="I46" s="36" t="s">
         <v>173</v>
       </c>
-      <c r="J46" s="33" t="s">
+      <c r="J46" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="K46" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="L46" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="M46" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="N46" s="34" t="s">
+      <c r="K46" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="L46" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="M46" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="N46" s="37" t="s">
         <v>238</v>
       </c>
-      <c r="O46" s="33" t="s">
+      <c r="O46" s="36" t="s">
         <v>239</v>
       </c>
-      <c r="P46" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q46" s="33" t="s">
+      <c r="P46" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q46" s="36" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="32" t="s">
+      <c r="A47" s="35" t="s">
         <v>240</v>
       </c>
-      <c r="B47" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="C47" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="D47" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="E47" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="F47" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="G47" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="H47" s="36" t="s">
+      <c r="B47" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="C47" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="D47" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="E47" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="F47" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="G47" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="H47" s="39" t="s">
         <v>138</v>
       </c>
-      <c r="I47" s="33" t="s">
+      <c r="I47" s="36" t="s">
         <v>179</v>
       </c>
-      <c r="J47" s="33" t="s">
+      <c r="J47" s="36" t="s">
         <v>241</v>
       </c>
-      <c r="K47" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="L47" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="M47" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="N47" s="34" t="s">
+      <c r="K47" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="L47" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="M47" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="N47" s="37" t="s">
         <v>242</v>
       </c>
-      <c r="O47" s="33" t="s">
+      <c r="O47" s="36" t="s">
         <v>243</v>
       </c>
-      <c r="P47" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q47" s="33" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="48" s="38" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="20" t="s">
+      <c r="P47" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q47" s="36" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="48" s="41" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="21" t="s">
         <v>244</v>
       </c>
-      <c r="B48" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="C48" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="D48" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="E48" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="F48" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="G48" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="H48" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="I48" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="J48" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="K48" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="L48" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="M48" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="N48" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="O48" s="37" t="s">
-        <v>32</v>
-      </c>
-      <c r="P48" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q48" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="R48" s="38" t="s">
+      <c r="B48" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="C48" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="D48" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="E48" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="F48" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="G48" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="H48" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="I48" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="J48" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="K48" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="L48" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="M48" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="N48" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="O48" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="P48" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q48" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="R48" s="41" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="49" s="38" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="20" t="s">
+    <row r="49" s="41" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="21" t="s">
         <v>246</v>
       </c>
-      <c r="B49" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="C49" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="D49" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="E49" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="F49" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="G49" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="H49" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="I49" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="J49" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="K49" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="L49" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="M49" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="N49" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="O49" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="P49" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q49" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="R49" s="38" t="s">
+      <c r="B49" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="C49" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="D49" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="E49" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="F49" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="G49" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="H49" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="I49" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="J49" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="K49" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="L49" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="M49" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="N49" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="O49" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="P49" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q49" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="R49" s="41" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="50" s="38" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="20" t="s">
+    <row r="50" s="41" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="21" t="s">
         <v>248</v>
       </c>
-      <c r="B50" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="C50" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="D50" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="E50" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="F50" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="G50" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="H50" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="I50" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="J50" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="K50" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="L50" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="M50" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="N50" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="O50" s="37" t="s">
-        <v>32</v>
-      </c>
-      <c r="P50" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q50" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="R50" s="38" t="s">
+      <c r="B50" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="C50" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="D50" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="E50" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="F50" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="G50" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="H50" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="I50" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="J50" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="K50" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="L50" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="M50" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="N50" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="O50" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="P50" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q50" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="R50" s="41" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="51" s="42" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="39" t="s">
+    <row r="51" s="45" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="42" t="s">
         <v>250</v>
       </c>
-      <c r="B51" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="C51" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="D51" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="E51" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="F51" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="G51" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="H51" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="I51" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="J51" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="K51" s="40" t="s">
+      <c r="B51" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="C51" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="D51" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="E51" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="F51" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="G51" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="H51" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="I51" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="J51" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="K51" s="43" t="s">
         <v>101</v>
       </c>
-      <c r="L51" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="M51" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="N51" s="41" t="s">
+      <c r="L51" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="M51" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="N51" s="44" t="s">
         <v>251</v>
       </c>
-      <c r="O51" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="P51" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q51" s="40" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="52" s="42" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="39" t="s">
+      <c r="O51" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="P51" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q51" s="43" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="52" s="45" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="42" t="s">
         <v>252</v>
       </c>
-      <c r="B52" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="C52" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="D52" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="E52" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="F52" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="G52" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="H52" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="I52" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="J52" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="K52" s="40" t="s">
+      <c r="B52" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="C52" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="D52" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="E52" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="F52" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="G52" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="H52" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="I52" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="J52" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="K52" s="43" t="s">
         <v>106</v>
       </c>
-      <c r="L52" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="M52" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="N52" s="41" t="s">
+      <c r="L52" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="M52" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="N52" s="44" t="s">
         <v>253</v>
       </c>
-      <c r="O52" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="P52" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q52" s="40" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="53" s="35" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="32" t="s">
+      <c r="O52" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="P52" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q52" s="43" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="53" s="38" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="35" t="s">
         <v>254</v>
       </c>
-      <c r="B53" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="C53" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="D53" s="33" t="s">
+      <c r="B53" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="C53" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="D53" s="36" t="s">
         <v>255</v>
       </c>
-      <c r="E53" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="F53" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="G53" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="H53" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="I53" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="J53" s="33" t="s">
+      <c r="E53" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="F53" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="G53" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="H53" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="I53" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="J53" s="36" t="s">
         <v>256</v>
       </c>
-      <c r="K53" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="L53" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="M53" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="N53" s="34" t="s">
+      <c r="K53" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="L53" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="M53" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="N53" s="37" t="s">
         <v>257</v>
       </c>
-      <c r="O53" s="33" t="s">
+      <c r="O53" s="36" t="s">
         <v>258</v>
       </c>
-      <c r="P53" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q53" s="33" t="s">
+      <c r="P53" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q53" s="36" t="s">
         <v>32</v>
       </c>
     </row>
@@ -4629,109 +4639,109 @@
         <v>32</v>
       </c>
     </row>
-    <row r="55" s="42" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="39" t="s">
+    <row r="55" s="45" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="42" t="s">
         <v>261</v>
       </c>
-      <c r="B55" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="C55" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="D55" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="E55" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="F55" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="G55" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="H55" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="I55" s="40" t="s">
+      <c r="B55" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="C55" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="D55" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="E55" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="F55" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="G55" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="H55" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="I55" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="J55" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="K55" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="L55" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="M55" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="N55" s="41" t="s">
+      <c r="J55" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="K55" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="L55" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="M55" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="N55" s="44" t="s">
         <v>262</v>
       </c>
-      <c r="O55" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="P55" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q55" s="40" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="56" s="42" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="39" t="s">
+      <c r="O55" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="P55" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q55" s="43" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="56" s="45" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="42" t="s">
         <v>263</v>
       </c>
-      <c r="B56" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="C56" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="D56" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="E56" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="F56" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="G56" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="H56" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="I56" s="40" t="s">
+      <c r="B56" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="C56" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="D56" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="E56" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="F56" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="G56" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="H56" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="I56" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="J56" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="K56" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="L56" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="M56" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="N56" s="41" t="s">
+      <c r="J56" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="K56" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="L56" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="M56" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="N56" s="44" t="s">
         <v>264</v>
       </c>
-      <c r="O56" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="P56" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q56" s="40" t="s">
+      <c r="O56" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="P56" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q56" s="43" t="s">
         <v>32</v>
       </c>
     </row>
@@ -4788,480 +4798,480 @@
         <v>32</v>
       </c>
     </row>
-    <row r="58" s="42" customFormat="true" ht="25.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="39" t="s">
+    <row r="58" s="45" customFormat="true" ht="25.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="42" t="s">
         <v>267</v>
       </c>
-      <c r="B58" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="C58" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="D58" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="E58" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="F58" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="G58" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="H58" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="I58" s="40" t="s">
+      <c r="B58" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="C58" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="D58" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="E58" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="F58" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="G58" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="H58" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="I58" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="J58" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="K58" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="L58" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="M58" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="N58" s="43" t="s">
+      <c r="J58" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="K58" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="L58" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="M58" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="N58" s="46" t="s">
         <v>268</v>
       </c>
-      <c r="O58" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="P58" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q58" s="40" t="s">
+      <c r="O58" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="P58" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q58" s="43" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="39" t="s">
+      <c r="A59" s="42" t="s">
         <v>269</v>
       </c>
-      <c r="B59" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="C59" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="D59" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="E59" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="F59" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="G59" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="H59" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="I59" s="40" t="s">
+      <c r="B59" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="C59" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="D59" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="E59" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="F59" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="G59" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="H59" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="I59" s="43" t="s">
         <v>168</v>
       </c>
-      <c r="J59" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="K59" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="L59" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="M59" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="N59" s="41" t="s">
+      <c r="J59" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="K59" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="L59" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="M59" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="N59" s="44" t="s">
         <v>270</v>
       </c>
-      <c r="O59" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="P59" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q59" s="40" t="s">
+      <c r="O59" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="P59" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q59" s="43" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="39" t="s">
+      <c r="A60" s="42" t="s">
         <v>271</v>
       </c>
-      <c r="B60" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="C60" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="D60" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="E60" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="F60" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="G60" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="H60" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="I60" s="40" t="s">
+      <c r="B60" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="C60" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="D60" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="E60" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="F60" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="G60" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="H60" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="I60" s="43" t="s">
         <v>173</v>
       </c>
-      <c r="J60" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="K60" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="L60" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="M60" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="N60" s="41" t="s">
+      <c r="J60" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="K60" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="L60" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="M60" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="N60" s="44" t="s">
         <v>272</v>
       </c>
-      <c r="O60" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="P60" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q60" s="40" t="s">
+      <c r="O60" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="P60" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q60" s="43" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="39" t="s">
+      <c r="A61" s="42" t="s">
         <v>273</v>
       </c>
-      <c r="B61" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="C61" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="D61" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="E61" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="F61" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="G61" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="H61" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="I61" s="40" t="s">
+      <c r="B61" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="C61" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="D61" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="E61" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="F61" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="G61" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="H61" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="I61" s="43" t="s">
         <v>179</v>
       </c>
-      <c r="J61" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="K61" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="L61" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="M61" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="N61" s="41" t="s">
+      <c r="J61" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="K61" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="L61" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="M61" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="N61" s="44" t="s">
         <v>274</v>
       </c>
-      <c r="O61" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="P61" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q61" s="40" t="s">
+      <c r="O61" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="P61" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q61" s="43" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="39" t="s">
+      <c r="A62" s="42" t="s">
         <v>275</v>
       </c>
-      <c r="B62" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="C62" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="D62" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="E62" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="F62" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="G62" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="H62" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="I62" s="40" t="s">
+      <c r="B62" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="C62" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="D62" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="E62" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="F62" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="G62" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="H62" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="I62" s="43" t="s">
         <v>184</v>
       </c>
-      <c r="J62" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="K62" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="L62" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="M62" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="N62" s="41" t="s">
+      <c r="J62" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="K62" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="L62" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="M62" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="N62" s="44" t="s">
         <v>276</v>
       </c>
-      <c r="O62" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="P62" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q62" s="40" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="63" s="46" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="44" t="s">
+      <c r="O62" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="P62" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q62" s="43" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="63" s="49" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="47" t="s">
         <v>277</v>
       </c>
-      <c r="B63" s="45" t="s">
-        <v>32</v>
-      </c>
-      <c r="C63" s="45" t="s">
-        <v>32</v>
-      </c>
-      <c r="D63" s="45" t="s">
+      <c r="B63" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="C63" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="D63" s="48" t="s">
         <v>144</v>
       </c>
-      <c r="E63" s="45" t="s">
-        <v>32</v>
-      </c>
-      <c r="F63" s="45" t="s">
-        <v>32</v>
-      </c>
-      <c r="G63" s="45" t="s">
-        <v>32</v>
-      </c>
-      <c r="H63" s="45" t="s">
-        <v>32</v>
-      </c>
-      <c r="I63" s="45" t="s">
+      <c r="E63" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="F63" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="G63" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="H63" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="I63" s="48" t="s">
         <v>190</v>
       </c>
-      <c r="J63" s="45" t="s">
-        <v>32</v>
-      </c>
-      <c r="K63" s="45" t="s">
-        <v>32</v>
-      </c>
-      <c r="L63" s="45" t="s">
-        <v>32</v>
-      </c>
-      <c r="M63" s="45" t="s">
-        <v>32</v>
-      </c>
-      <c r="N63" s="45" t="s">
+      <c r="J63" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="K63" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="L63" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="M63" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="N63" s="48" t="s">
         <v>278</v>
       </c>
-      <c r="O63" s="45" t="s">
-        <v>32</v>
-      </c>
-      <c r="P63" s="45" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q63" s="45" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="64" s="46" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="44" t="s">
+      <c r="O63" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="P63" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q63" s="48" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="64" s="49" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="47" t="s">
         <v>279</v>
       </c>
-      <c r="B64" s="45" t="s">
-        <v>32</v>
-      </c>
-      <c r="C64" s="45" t="s">
-        <v>32</v>
-      </c>
-      <c r="D64" s="45" t="s">
+      <c r="B64" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="C64" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="D64" s="48" t="s">
         <v>149</v>
       </c>
-      <c r="E64" s="45" t="s">
-        <v>32</v>
-      </c>
-      <c r="F64" s="45" t="s">
-        <v>32</v>
-      </c>
-      <c r="G64" s="45" t="s">
-        <v>32</v>
-      </c>
-      <c r="H64" s="45" t="s">
-        <v>32</v>
-      </c>
-      <c r="I64" s="45" t="s">
-        <v>32</v>
-      </c>
-      <c r="J64" s="45" t="s">
-        <v>32</v>
-      </c>
-      <c r="K64" s="45" t="s">
-        <v>32</v>
-      </c>
-      <c r="L64" s="45" t="s">
-        <v>32</v>
-      </c>
-      <c r="M64" s="45" t="s">
-        <v>32</v>
-      </c>
-      <c r="N64" s="45" t="s">
+      <c r="E64" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="F64" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="G64" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="H64" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="I64" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="J64" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="K64" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="L64" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="M64" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="N64" s="48" t="s">
         <v>280</v>
       </c>
-      <c r="O64" s="45" t="s">
-        <v>32</v>
-      </c>
-      <c r="P64" s="45" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q64" s="45" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="65" s="42" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="39" t="s">
+      <c r="O64" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="P64" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q64" s="48" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="65" s="45" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="42" t="s">
         <v>281</v>
       </c>
-      <c r="B65" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="C65" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="D65" s="40" t="s">
+      <c r="B65" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="C65" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="D65" s="43" t="s">
         <v>154</v>
       </c>
-      <c r="E65" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="F65" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="G65" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="H65" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="I65" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="J65" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="K65" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="L65" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="M65" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="N65" s="41" t="s">
+      <c r="E65" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="F65" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="G65" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="H65" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="I65" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="J65" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="K65" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="L65" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="M65" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="N65" s="44" t="s">
         <v>282</v>
       </c>
-      <c r="O65" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="P65" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q65" s="40" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="66" s="42" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="39" t="s">
+      <c r="O65" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="P65" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q65" s="43" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="66" s="45" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="42" t="s">
         <v>283</v>
       </c>
-      <c r="B66" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="C66" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="D66" s="40" t="s">
+      <c r="B66" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="C66" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="D66" s="43" t="s">
         <v>160</v>
       </c>
-      <c r="E66" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="F66" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="G66" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="H66" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="I66" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="J66" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="K66" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="L66" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="M66" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="N66" s="41" t="s">
+      <c r="E66" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="F66" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="G66" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="H66" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="I66" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="J66" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="K66" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="L66" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="M66" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="N66" s="44" t="s">
         <v>284</v>
       </c>
-      <c r="O66" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="P66" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q66" s="40" t="s">
+      <c r="O66" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="P66" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q66" s="43" t="s">
         <v>32</v>
       </c>
     </row>
@@ -5636,480 +5646,480 @@
         <v>32</v>
       </c>
     </row>
-    <row r="74" s="42" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="39" t="s">
+    <row r="74" s="45" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="42" t="s">
         <v>305</v>
       </c>
-      <c r="B74" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="C74" s="40" t="s">
+      <c r="B74" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="C74" s="43" t="s">
         <v>104</v>
       </c>
-      <c r="D74" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="E74" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="F74" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="G74" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="H74" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="I74" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="J74" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="K74" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="L74" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="M74" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="N74" s="41" t="s">
+      <c r="D74" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="E74" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="F74" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="G74" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="H74" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="I74" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="J74" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="K74" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="L74" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="M74" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="N74" s="44" t="s">
         <v>306</v>
       </c>
-      <c r="O74" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="P74" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q74" s="40" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="75" s="42" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="39" t="s">
+      <c r="O74" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="P74" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q74" s="43" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="75" s="45" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="42" t="s">
         <v>307</v>
       </c>
-      <c r="B75" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="C75" s="40" t="s">
+      <c r="B75" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="C75" s="43" t="s">
         <v>77</v>
       </c>
-      <c r="D75" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="E75" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="F75" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="G75" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="H75" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="I75" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="J75" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="K75" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="L75" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="M75" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="N75" s="41" t="s">
+      <c r="D75" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="E75" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="F75" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="G75" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="H75" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="I75" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="J75" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="K75" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="L75" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="M75" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="N75" s="44" t="s">
         <v>308</v>
       </c>
-      <c r="O75" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="P75" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q75" s="40" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="76" s="42" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="39" t="s">
+      <c r="O75" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="P75" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q75" s="43" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="76" s="45" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="42" t="s">
         <v>309</v>
       </c>
-      <c r="B76" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="C76" s="40" t="s">
+      <c r="B76" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="C76" s="43" t="s">
         <v>84</v>
       </c>
-      <c r="D76" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="E76" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="F76" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="G76" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="H76" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="I76" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="J76" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="K76" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="L76" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="M76" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="N76" s="41" t="s">
+      <c r="D76" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="E76" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="F76" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="G76" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="H76" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="I76" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="J76" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="K76" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="L76" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="M76" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="N76" s="44" t="s">
         <v>310</v>
       </c>
-      <c r="O76" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="P76" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q76" s="40" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="77" s="42" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="39" t="s">
+      <c r="O76" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="P76" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q76" s="43" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="77" s="45" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="42" t="s">
         <v>311</v>
       </c>
-      <c r="B77" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="C77" s="40" t="s">
+      <c r="B77" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="C77" s="43" t="s">
         <v>117</v>
       </c>
-      <c r="D77" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="E77" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="F77" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="G77" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="H77" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="I77" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="J77" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="K77" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="L77" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="M77" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="N77" s="41" t="s">
+      <c r="D77" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="E77" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="F77" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="G77" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="H77" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="I77" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="J77" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="K77" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="L77" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="M77" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="N77" s="44" t="s">
         <v>312</v>
       </c>
-      <c r="O77" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="P77" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q77" s="40" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="78" s="42" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="39" t="s">
+      <c r="O77" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="P77" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q77" s="43" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="78" s="45" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="42" t="s">
         <v>313</v>
       </c>
-      <c r="B78" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="C78" s="40" t="s">
+      <c r="B78" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="C78" s="43" t="s">
         <v>89</v>
       </c>
-      <c r="D78" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="E78" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="F78" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="G78" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="H78" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="I78" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="J78" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="K78" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="L78" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="M78" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="N78" s="41" t="s">
+      <c r="D78" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="E78" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="F78" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="G78" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="H78" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="I78" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="J78" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="K78" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="L78" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="M78" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="N78" s="44" t="s">
         <v>314</v>
       </c>
-      <c r="O78" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="P78" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q78" s="40" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="79" s="42" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="39" t="s">
+      <c r="O78" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="P78" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q78" s="43" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="79" s="45" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="42" t="s">
         <v>315</v>
       </c>
-      <c r="B79" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="C79" s="40" t="s">
+      <c r="B79" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="C79" s="43" t="s">
         <v>123</v>
       </c>
-      <c r="D79" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="E79" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="F79" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="G79" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="H79" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="I79" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="J79" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="K79" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="L79" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="M79" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="N79" s="41" t="s">
+      <c r="D79" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="E79" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="F79" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="G79" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="H79" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="I79" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="J79" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="K79" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="L79" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="M79" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="N79" s="44" t="s">
         <v>316</v>
       </c>
-      <c r="O79" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="P79" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q79" s="40" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="80" s="42" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="39" t="s">
+      <c r="O79" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="P79" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q79" s="43" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="80" s="45" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="42" t="s">
         <v>317</v>
       </c>
-      <c r="B80" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="C80" s="40" t="s">
+      <c r="B80" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="C80" s="43" t="s">
         <v>94</v>
       </c>
-      <c r="D80" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="E80" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="F80" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="G80" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="H80" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="I80" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="J80" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="K80" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="L80" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="M80" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="N80" s="41" t="s">
+      <c r="D80" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="E80" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="F80" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="G80" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="H80" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="I80" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="J80" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="K80" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="L80" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="M80" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="N80" s="44" t="s">
         <v>318</v>
       </c>
-      <c r="O80" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="P80" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q80" s="40" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="81" s="42" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="39" t="s">
+      <c r="O80" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="P80" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q80" s="43" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="81" s="45" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="42" t="s">
         <v>319</v>
       </c>
-      <c r="B81" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="C81" s="40" t="s">
+      <c r="B81" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="C81" s="43" t="s">
         <v>99</v>
       </c>
-      <c r="D81" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="E81" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="F81" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="G81" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="H81" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="I81" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="J81" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="K81" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="L81" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="M81" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="N81" s="41" t="s">
+      <c r="D81" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="E81" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="F81" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="G81" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="H81" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="I81" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="J81" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="K81" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="L81" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="M81" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="N81" s="44" t="s">
         <v>320</v>
       </c>
-      <c r="O81" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="P81" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q81" s="40" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="82" s="42" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="39" t="s">
+      <c r="O81" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="P81" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q81" s="43" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="82" s="45" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="42" t="s">
         <v>321</v>
       </c>
-      <c r="B82" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="C82" s="40" t="s">
+      <c r="B82" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="C82" s="43" t="s">
         <v>70</v>
       </c>
-      <c r="D82" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="E82" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="F82" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="G82" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="H82" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="I82" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="J82" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="K82" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="L82" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="M82" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="N82" s="41" t="s">
+      <c r="D82" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="E82" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="F82" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="G82" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="H82" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="I82" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="J82" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="K82" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="L82" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="M82" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="N82" s="44" t="s">
         <v>322</v>
       </c>
-      <c r="O82" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="P82" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q82" s="40" t="s">
+      <c r="O82" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="P82" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q82" s="43" t="s">
         <v>32</v>
       </c>
     </row>
@@ -7728,7 +7738,7 @@
         <v>32</v>
       </c>
       <c r="J113" s="6" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="K113" s="6" t="s">
         <v>32</v>
@@ -8535,7 +8545,7 @@
       <c r="N128" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="O128" s="47" t="s">
+      <c r="O128" s="50" t="s">
         <v>32</v>
       </c>
       <c r="P128" s="6" t="s">
@@ -8930,7 +8940,7 @@
         <v>32</v>
       </c>
       <c r="E136" s="6" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="F136" s="6" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
stm32f4_function_mappings.xlsx: update NRF24 function mapping
</commit_message>
<xml_diff>
--- a/platform/embedded/stm32f407/stm32f4_function_mappings.xlsx
+++ b/platform/embedded/stm32f407/stm32f4_function_mappings.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2404" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2405" uniqueCount="423">
   <si>
     <t xml:space="preserve">Port</t>
   </si>
@@ -667,6 +667,9 @@
   <si>
     <t xml:space="preserve">OTG_HS_ULPI_
 STP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SDIO_CD</t>
   </si>
   <si>
     <t xml:space="preserve">PC1</t>
@@ -1420,14 +1423,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00FFFF"/>
-        <bgColor rgb="FF00FFFF"/>
+        <fgColor rgb="FFFF33FF"/>
+        <bgColor rgb="FFFF00FF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF33FF"/>
-        <bgColor rgb="FFFF00FF"/>
+        <fgColor rgb="FF00FFFF"/>
+        <bgColor rgb="FF00FFFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -1477,7 +1480,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1598,10 +1601,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1610,12 +1609,16 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1634,7 +1637,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1762,11 +1769,11 @@
   <dimension ref="A1:R142"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B32" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
-      <selection pane="bottomRight" activeCell="M40" activeCellId="0" sqref="M40"/>
+      <selection pane="bottomLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
+      <selection pane="bottomRight" activeCell="R48" activeCellId="0" sqref="R48:R50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3572,62 +3579,65 @@
         <v>32</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="5" t="s">
+    <row r="35" s="33" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="30" t="s">
         <v>198</v>
       </c>
-      <c r="B35" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D35" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E35" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F35" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G35" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="H35" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="I35" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="J35" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="K35" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="L35" s="7" t="s">
+      <c r="B35" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="C35" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="D35" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="E35" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="F35" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="G35" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="H35" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="I35" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="J35" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="K35" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="L35" s="32" t="s">
         <v>199</v>
       </c>
-      <c r="M35" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="N35" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="O35" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="P35" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q35" s="6" t="s">
-        <v>32</v>
+      <c r="M35" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="N35" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="O35" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="P35" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q35" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="R35" s="30" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="36" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="8" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B36" s="9" t="s">
         <v>32</v>
@@ -3663,7 +3673,7 @@
         <v>32</v>
       </c>
       <c r="M36" s="12" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="N36" s="9" t="s">
         <v>32</v>
@@ -3680,7 +3690,7 @@
     </row>
     <row r="37" s="20" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="18" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B37" s="19" t="s">
         <v>32</v>
@@ -3697,7 +3707,7 @@
       <c r="F37" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="G37" s="30" t="s">
+      <c r="G37" s="34" t="s">
         <v>188</v>
       </c>
       <c r="H37" s="19" t="s">
@@ -3713,10 +3723,10 @@
         <v>32</v>
       </c>
       <c r="L37" s="28" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="M37" s="19" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="N37" s="19" t="s">
         <v>32</v>
@@ -3733,7 +3743,7 @@
     </row>
     <row r="38" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="5" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B38" s="6" t="s">
         <v>32</v>
@@ -3766,10 +3776,10 @@
         <v>32</v>
       </c>
       <c r="L38" s="7" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="M38" s="7" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="N38" s="6" t="s">
         <v>32</v>
@@ -3786,7 +3796,7 @@
     </row>
     <row r="39" s="11" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="8" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B39" s="9" t="s">
         <v>32</v>
@@ -3839,7 +3849,7 @@
     </row>
     <row r="40" s="11" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="8" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B40" s="9" t="s">
         <v>32</v>
@@ -3875,7 +3885,7 @@
         <v>32</v>
       </c>
       <c r="M40" s="10" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="N40" s="9" t="s">
         <v>32</v>
@@ -3890,378 +3900,378 @@
         <v>32</v>
       </c>
     </row>
-    <row r="41" s="34" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="31" t="s">
-        <v>211</v>
-      </c>
-      <c r="B41" s="32" t="s">
-        <v>32</v>
-      </c>
-      <c r="C41" s="32" t="s">
-        <v>32</v>
-      </c>
-      <c r="D41" s="32" t="s">
+    <row r="41" s="38" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="35" t="s">
         <v>212</v>
       </c>
-      <c r="E41" s="32" t="s">
-        <v>212</v>
-      </c>
-      <c r="F41" s="32" t="s">
-        <v>32</v>
-      </c>
-      <c r="G41" s="32" t="s">
+      <c r="B41" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="C41" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="D41" s="36" t="s">
         <v>213</v>
       </c>
-      <c r="H41" s="32" t="s">
-        <v>32</v>
-      </c>
-      <c r="I41" s="32" t="s">
-        <v>32</v>
-      </c>
-      <c r="J41" s="33" t="s">
+      <c r="E41" s="36" t="s">
+        <v>213</v>
+      </c>
+      <c r="F41" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="G41" s="36" t="s">
         <v>214</v>
       </c>
-      <c r="K41" s="32" t="s">
-        <v>32</v>
-      </c>
-      <c r="L41" s="32" t="s">
-        <v>32</v>
-      </c>
-      <c r="M41" s="32"/>
-      <c r="N41" s="32" t="s">
+      <c r="H41" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="I41" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="J41" s="37" t="s">
         <v>215</v>
       </c>
-      <c r="O41" s="32" t="s">
+      <c r="K41" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="L41" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="M41" s="36"/>
+      <c r="N41" s="36" t="s">
+        <v>216</v>
+      </c>
+      <c r="O41" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="P41" s="32" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q41" s="32" t="s">
+      <c r="P41" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q41" s="36" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="31" t="s">
-        <v>216</v>
-      </c>
-      <c r="B42" s="32" t="s">
-        <v>32</v>
-      </c>
-      <c r="C42" s="32" t="s">
-        <v>32</v>
-      </c>
-      <c r="D42" s="32" t="s">
+      <c r="A42" s="35" t="s">
         <v>217</v>
       </c>
-      <c r="E42" s="32" t="s">
-        <v>217</v>
-      </c>
-      <c r="F42" s="32" t="s">
-        <v>32</v>
-      </c>
-      <c r="G42" s="32" t="s">
-        <v>32</v>
-      </c>
-      <c r="H42" s="32" t="s">
+      <c r="B42" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="C42" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="D42" s="36" t="s">
         <v>218</v>
       </c>
-      <c r="I42" s="32" t="s">
-        <v>32</v>
-      </c>
-      <c r="J42" s="33" t="s">
+      <c r="E42" s="36" t="s">
+        <v>218</v>
+      </c>
+      <c r="F42" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="G42" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="H42" s="36" t="s">
         <v>219</v>
       </c>
-      <c r="K42" s="32" t="s">
-        <v>32</v>
-      </c>
-      <c r="L42" s="32" t="s">
-        <v>32</v>
-      </c>
-      <c r="M42" s="32" t="s">
-        <v>32</v>
-      </c>
-      <c r="N42" s="32" t="s">
+      <c r="I42" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="J42" s="37" t="s">
         <v>220</v>
       </c>
-      <c r="O42" s="32" t="s">
+      <c r="K42" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="L42" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="M42" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="N42" s="36" t="s">
+        <v>221</v>
+      </c>
+      <c r="O42" s="36" t="s">
         <v>97</v>
       </c>
-      <c r="P42" s="32" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q42" s="32" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="43" s="38" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="35" t="s">
-        <v>221</v>
-      </c>
-      <c r="B43" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="C43" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="D43" s="36" t="s">
+      <c r="P42" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q42" s="36" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="43" s="33" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="30" t="s">
         <v>222</v>
       </c>
-      <c r="E43" s="36" t="s">
-        <v>222</v>
-      </c>
-      <c r="F43" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="G43" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="H43" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="I43" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="J43" s="36" t="s">
+      <c r="B43" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="C43" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="D43" s="31" t="s">
         <v>223</v>
       </c>
-      <c r="K43" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="L43" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="M43" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="N43" s="37" t="s">
+      <c r="E43" s="31" t="s">
+        <v>223</v>
+      </c>
+      <c r="F43" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="G43" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="H43" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="I43" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="J43" s="31" t="s">
         <v>224</v>
       </c>
-      <c r="O43" s="36" t="s">
+      <c r="K43" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="L43" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="M43" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="N43" s="39" t="s">
         <v>225</v>
       </c>
-      <c r="P43" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q43" s="36" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="44" s="38" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="35" t="s">
+      <c r="O43" s="31" t="s">
         <v>226</v>
       </c>
-      <c r="B44" s="36" t="s">
+      <c r="P43" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q43" s="31" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="44" s="33" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="30" t="s">
         <v>227</v>
       </c>
-      <c r="C44" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="D44" s="36" t="s">
+      <c r="B44" s="31" t="s">
         <v>228</v>
       </c>
-      <c r="E44" s="36" t="s">
-        <v>228</v>
-      </c>
-      <c r="F44" s="36" t="s">
+      <c r="C44" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="D44" s="31" t="s">
         <v>229</v>
       </c>
-      <c r="G44" s="36" t="s">
+      <c r="E44" s="31" t="s">
+        <v>229</v>
+      </c>
+      <c r="F44" s="31" t="s">
         <v>230</v>
       </c>
-      <c r="H44" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="I44" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="J44" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="K44" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="L44" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="M44" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="N44" s="37" t="s">
+      <c r="G44" s="31" t="s">
         <v>231</v>
       </c>
-      <c r="O44" s="36" t="s">
+      <c r="H44" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="I44" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="J44" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="K44" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="L44" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="M44" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="N44" s="39" t="s">
         <v>232</v>
       </c>
-      <c r="P44" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q44" s="36" t="s">
+      <c r="O44" s="31" t="s">
+        <v>233</v>
+      </c>
+      <c r="P44" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q44" s="31" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="35" t="s">
-        <v>233</v>
-      </c>
-      <c r="B45" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="C45" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="D45" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="E45" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="F45" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="G45" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="H45" s="39" t="s">
+      <c r="A45" s="30" t="s">
         <v>234</v>
       </c>
-      <c r="I45" s="36" t="s">
+      <c r="B45" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="C45" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="D45" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="E45" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="F45" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="G45" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="H45" s="40" t="s">
+        <v>235</v>
+      </c>
+      <c r="I45" s="31" t="s">
         <v>168</v>
       </c>
-      <c r="J45" s="36" t="s">
+      <c r="J45" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="K45" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="L45" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="M45" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="N45" s="37" t="s">
-        <v>235</v>
-      </c>
-      <c r="O45" s="36" t="s">
+      <c r="K45" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="L45" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="M45" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="N45" s="39" t="s">
         <v>236</v>
       </c>
-      <c r="P45" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q45" s="36" t="s">
+      <c r="O45" s="31" t="s">
+        <v>237</v>
+      </c>
+      <c r="P45" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q45" s="31" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="35" t="s">
-        <v>237</v>
-      </c>
-      <c r="B46" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="C46" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="D46" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="E46" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="F46" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="G46" s="36" t="s">
+      <c r="A46" s="30" t="s">
+        <v>238</v>
+      </c>
+      <c r="B46" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="C46" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="D46" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="E46" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="F46" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="G46" s="31" t="s">
         <v>135</v>
       </c>
-      <c r="H46" s="37" t="s">
+      <c r="H46" s="39" t="s">
         <v>134</v>
       </c>
-      <c r="I46" s="36" t="s">
+      <c r="I46" s="31" t="s">
         <v>173</v>
       </c>
-      <c r="J46" s="36" t="s">
+      <c r="J46" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="K46" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="L46" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="M46" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="N46" s="37" t="s">
-        <v>238</v>
-      </c>
-      <c r="O46" s="36" t="s">
+      <c r="K46" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="L46" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="M46" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="N46" s="39" t="s">
         <v>239</v>
       </c>
-      <c r="P46" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q46" s="36" t="s">
+      <c r="O46" s="31" t="s">
+        <v>240</v>
+      </c>
+      <c r="P46" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q46" s="31" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="35" t="s">
-        <v>240</v>
-      </c>
-      <c r="B47" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="C47" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="D47" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="E47" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="F47" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="G47" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="H47" s="39" t="s">
+      <c r="A47" s="30" t="s">
+        <v>241</v>
+      </c>
+      <c r="B47" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="C47" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="D47" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="E47" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="F47" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="G47" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="H47" s="40" t="s">
         <v>138</v>
       </c>
-      <c r="I47" s="36" t="s">
+      <c r="I47" s="31" t="s">
         <v>179</v>
       </c>
-      <c r="J47" s="36" t="s">
-        <v>241</v>
-      </c>
-      <c r="K47" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="L47" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="M47" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="N47" s="37" t="s">
+      <c r="J47" s="31" t="s">
         <v>242</v>
       </c>
-      <c r="O47" s="36" t="s">
+      <c r="K47" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="L47" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="M47" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="N47" s="39" t="s">
         <v>243</v>
       </c>
-      <c r="P47" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q47" s="36" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="48" s="41" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O47" s="31" t="s">
+        <v>244</v>
+      </c>
+      <c r="P47" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q47" s="31" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="48" s="42" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="21" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B48" s="23" t="s">
         <v>32</v>
@@ -4302,7 +4312,7 @@
       <c r="N48" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="O48" s="40" t="s">
+      <c r="O48" s="41" t="s">
         <v>32</v>
       </c>
       <c r="P48" s="23" t="s">
@@ -4311,13 +4321,13 @@
       <c r="Q48" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="R48" s="41" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="49" s="41" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R48" s="21" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="49" s="42" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="21" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B49" s="23" t="s">
         <v>32</v>
@@ -4367,13 +4377,13 @@
       <c r="Q49" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="R49" s="41" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="50" s="41" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R49" s="21" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="50" s="42" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="21" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B50" s="23" t="s">
         <v>32</v>
@@ -4414,7 +4424,7 @@
       <c r="N50" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="O50" s="40" t="s">
+      <c r="O50" s="41" t="s">
         <v>32</v>
       </c>
       <c r="P50" s="23" t="s">
@@ -4423,172 +4433,172 @@
       <c r="Q50" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="R50" s="41" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="51" s="45" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="42" t="s">
+      <c r="R50" s="21" t="s">
         <v>250</v>
       </c>
-      <c r="B51" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="C51" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="D51" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="E51" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="F51" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="G51" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="H51" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="I51" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="J51" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="K51" s="43" t="s">
+    </row>
+    <row r="51" s="46" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="43" t="s">
+        <v>251</v>
+      </c>
+      <c r="B51" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="C51" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="D51" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="E51" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="F51" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="G51" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="H51" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="I51" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="J51" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="K51" s="44" t="s">
         <v>101</v>
       </c>
-      <c r="L51" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="M51" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="N51" s="44" t="s">
-        <v>251</v>
-      </c>
-      <c r="O51" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="P51" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q51" s="43" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="52" s="45" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="42" t="s">
+      <c r="L51" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="M51" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="N51" s="45" t="s">
         <v>252</v>
       </c>
-      <c r="B52" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="C52" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="D52" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="E52" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="F52" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="G52" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="H52" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="I52" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="J52" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="K52" s="43" t="s">
+      <c r="O51" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="P51" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q51" s="44" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="52" s="46" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="43" t="s">
+        <v>253</v>
+      </c>
+      <c r="B52" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="C52" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="D52" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="E52" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="F52" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="G52" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="H52" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="I52" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="J52" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="K52" s="44" t="s">
         <v>106</v>
       </c>
-      <c r="L52" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="M52" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="N52" s="44" t="s">
-        <v>253</v>
-      </c>
-      <c r="O52" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="P52" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q52" s="43" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="53" s="38" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="35" t="s">
+      <c r="L52" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="M52" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="N52" s="45" t="s">
         <v>254</v>
       </c>
-      <c r="B53" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="C53" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="D53" s="36" t="s">
+      <c r="O52" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="P52" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q52" s="44" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="53" s="33" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="30" t="s">
         <v>255</v>
       </c>
-      <c r="E53" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="F53" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="G53" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="H53" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="I53" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="J53" s="36" t="s">
+      <c r="B53" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="C53" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="D53" s="31" t="s">
         <v>256</v>
       </c>
-      <c r="K53" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="L53" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="M53" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="N53" s="37" t="s">
+      <c r="E53" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="F53" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="G53" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="H53" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="I53" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="J53" s="31" t="s">
         <v>257</v>
       </c>
-      <c r="O53" s="36" t="s">
+      <c r="K53" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="L53" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="M53" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="N53" s="39" t="s">
         <v>258</v>
       </c>
-      <c r="P53" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q53" s="36" t="s">
+      <c r="O53" s="31" t="s">
+        <v>259</v>
+      </c>
+      <c r="P53" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q53" s="31" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="5" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B54" s="6" t="s">
         <v>32</v>
@@ -4627,7 +4637,7 @@
         <v>32</v>
       </c>
       <c r="N54" s="6" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="O54" s="6" t="s">
         <v>32</v>
@@ -4639,115 +4649,115 @@
         <v>32</v>
       </c>
     </row>
-    <row r="55" s="45" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="42" t="s">
-        <v>261</v>
-      </c>
-      <c r="B55" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="C55" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="D55" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="E55" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="F55" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="G55" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="H55" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="I55" s="43" t="s">
+    <row r="55" s="46" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="43" t="s">
+        <v>262</v>
+      </c>
+      <c r="B55" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="C55" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="D55" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="E55" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="F55" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="G55" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="H55" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="I55" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="J55" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="K55" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="L55" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="M55" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="N55" s="44" t="s">
-        <v>262</v>
-      </c>
-      <c r="O55" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="P55" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q55" s="43" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="56" s="45" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="42" t="s">
+      <c r="J55" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="K55" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="L55" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="M55" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="N55" s="45" t="s">
         <v>263</v>
       </c>
-      <c r="B56" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="C56" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="D56" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="E56" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="F56" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="G56" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="H56" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="I56" s="43" t="s">
+      <c r="O55" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="P55" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q55" s="44" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="56" s="46" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="43" t="s">
+        <v>264</v>
+      </c>
+      <c r="B56" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="C56" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="D56" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="E56" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="F56" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="G56" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="H56" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="I56" s="44" t="s">
         <v>49</v>
       </c>
-      <c r="J56" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="K56" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="L56" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="M56" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="N56" s="44" t="s">
-        <v>264</v>
-      </c>
-      <c r="O56" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="P56" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q56" s="43" t="s">
+      <c r="J56" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="K56" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="L56" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="M56" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="N56" s="45" t="s">
+        <v>265</v>
+      </c>
+      <c r="O56" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="P56" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q56" s="44" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="5" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B57" s="6" t="s">
         <v>32</v>
@@ -4786,7 +4796,7 @@
         <v>32</v>
       </c>
       <c r="N57" s="6" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="O57" s="6" t="s">
         <v>32</v>
@@ -4798,486 +4808,486 @@
         <v>32</v>
       </c>
     </row>
-    <row r="58" s="45" customFormat="true" ht="25.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="42" t="s">
-        <v>267</v>
-      </c>
-      <c r="B58" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="C58" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="D58" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="E58" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="F58" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="G58" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="H58" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="I58" s="43" t="s">
+    <row r="58" s="46" customFormat="true" ht="25.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="43" t="s">
+        <v>268</v>
+      </c>
+      <c r="B58" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="C58" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="D58" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="E58" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="F58" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="G58" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="H58" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="I58" s="44" t="s">
         <v>61</v>
       </c>
-      <c r="J58" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="K58" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="L58" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="M58" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="N58" s="46" t="s">
-        <v>268</v>
-      </c>
-      <c r="O58" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="P58" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q58" s="43" t="s">
+      <c r="J58" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="K58" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="L58" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="M58" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="N58" s="47" t="s">
+        <v>269</v>
+      </c>
+      <c r="O58" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="P58" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q58" s="44" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="42" t="s">
-        <v>269</v>
-      </c>
-      <c r="B59" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="C59" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="D59" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="E59" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="F59" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="G59" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="H59" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="I59" s="43" t="s">
+      <c r="A59" s="43" t="s">
+        <v>270</v>
+      </c>
+      <c r="B59" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="C59" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="D59" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="E59" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="F59" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="G59" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="H59" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="I59" s="44" t="s">
         <v>168</v>
       </c>
-      <c r="J59" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="K59" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="L59" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="M59" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="N59" s="44" t="s">
-        <v>270</v>
-      </c>
-      <c r="O59" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="P59" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q59" s="43" t="s">
+      <c r="J59" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="K59" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="L59" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="M59" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="N59" s="45" t="s">
+        <v>271</v>
+      </c>
+      <c r="O59" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="P59" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q59" s="44" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="42" t="s">
-        <v>271</v>
-      </c>
-      <c r="B60" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="C60" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="D60" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="E60" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="F60" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="G60" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="H60" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="I60" s="43" t="s">
+      <c r="A60" s="43" t="s">
+        <v>272</v>
+      </c>
+      <c r="B60" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="C60" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="D60" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="E60" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="F60" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="G60" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="H60" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="I60" s="44" t="s">
         <v>173</v>
       </c>
-      <c r="J60" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="K60" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="L60" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="M60" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="N60" s="44" t="s">
-        <v>272</v>
-      </c>
-      <c r="O60" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="P60" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q60" s="43" t="s">
+      <c r="J60" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="K60" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="L60" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="M60" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="N60" s="45" t="s">
+        <v>273</v>
+      </c>
+      <c r="O60" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="P60" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q60" s="44" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="42" t="s">
-        <v>273</v>
-      </c>
-      <c r="B61" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="C61" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="D61" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="E61" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="F61" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="G61" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="H61" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="I61" s="43" t="s">
+      <c r="A61" s="43" t="s">
+        <v>274</v>
+      </c>
+      <c r="B61" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="C61" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="D61" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="E61" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="F61" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="G61" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="H61" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="I61" s="44" t="s">
         <v>179</v>
       </c>
-      <c r="J61" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="K61" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="L61" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="M61" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="N61" s="44" t="s">
-        <v>274</v>
-      </c>
-      <c r="O61" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="P61" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q61" s="43" t="s">
+      <c r="J61" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="K61" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="L61" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="M61" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="N61" s="45" t="s">
+        <v>275</v>
+      </c>
+      <c r="O61" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="P61" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q61" s="44" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="42" t="s">
-        <v>275</v>
-      </c>
-      <c r="B62" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="C62" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="D62" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="E62" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="F62" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="G62" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="H62" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="I62" s="43" t="s">
+      <c r="A62" s="43" t="s">
+        <v>276</v>
+      </c>
+      <c r="B62" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="C62" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="D62" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="E62" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="F62" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="G62" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="H62" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="I62" s="44" t="s">
         <v>184</v>
       </c>
-      <c r="J62" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="K62" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="L62" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="M62" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="N62" s="44" t="s">
-        <v>276</v>
-      </c>
-      <c r="O62" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="P62" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q62" s="43" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="63" s="49" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="47" t="s">
+      <c r="J62" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="K62" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="L62" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="M62" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="N62" s="45" t="s">
         <v>277</v>
       </c>
-      <c r="B63" s="48" t="s">
-        <v>32</v>
-      </c>
-      <c r="C63" s="48" t="s">
-        <v>32</v>
-      </c>
-      <c r="D63" s="48" t="s">
+      <c r="O62" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="P62" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q62" s="44" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="63" s="50" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="48" t="s">
+        <v>278</v>
+      </c>
+      <c r="B63" s="49" t="s">
+        <v>32</v>
+      </c>
+      <c r="C63" s="49" t="s">
+        <v>32</v>
+      </c>
+      <c r="D63" s="49" t="s">
         <v>144</v>
       </c>
-      <c r="E63" s="48" t="s">
-        <v>32</v>
-      </c>
-      <c r="F63" s="48" t="s">
-        <v>32</v>
-      </c>
-      <c r="G63" s="48" t="s">
-        <v>32</v>
-      </c>
-      <c r="H63" s="48" t="s">
-        <v>32</v>
-      </c>
-      <c r="I63" s="48" t="s">
+      <c r="E63" s="49" t="s">
+        <v>32</v>
+      </c>
+      <c r="F63" s="49" t="s">
+        <v>32</v>
+      </c>
+      <c r="G63" s="49" t="s">
+        <v>32</v>
+      </c>
+      <c r="H63" s="49" t="s">
+        <v>32</v>
+      </c>
+      <c r="I63" s="49" t="s">
         <v>190</v>
       </c>
-      <c r="J63" s="48" t="s">
-        <v>32</v>
-      </c>
-      <c r="K63" s="48" t="s">
-        <v>32</v>
-      </c>
-      <c r="L63" s="48" t="s">
-        <v>32</v>
-      </c>
-      <c r="M63" s="48" t="s">
-        <v>32</v>
-      </c>
-      <c r="N63" s="48" t="s">
-        <v>278</v>
-      </c>
-      <c r="O63" s="48" t="s">
-        <v>32</v>
-      </c>
-      <c r="P63" s="48" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q63" s="48" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="64" s="49" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="47" t="s">
+      <c r="J63" s="49" t="s">
+        <v>32</v>
+      </c>
+      <c r="K63" s="49" t="s">
+        <v>32</v>
+      </c>
+      <c r="L63" s="49" t="s">
+        <v>32</v>
+      </c>
+      <c r="M63" s="49" t="s">
+        <v>32</v>
+      </c>
+      <c r="N63" s="49" t="s">
         <v>279</v>
       </c>
-      <c r="B64" s="48" t="s">
-        <v>32</v>
-      </c>
-      <c r="C64" s="48" t="s">
-        <v>32</v>
-      </c>
-      <c r="D64" s="48" t="s">
+      <c r="O63" s="49" t="s">
+        <v>32</v>
+      </c>
+      <c r="P63" s="49" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q63" s="49" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="64" s="50" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="48" t="s">
+        <v>280</v>
+      </c>
+      <c r="B64" s="49" t="s">
+        <v>32</v>
+      </c>
+      <c r="C64" s="49" t="s">
+        <v>32</v>
+      </c>
+      <c r="D64" s="49" t="s">
         <v>149</v>
       </c>
-      <c r="E64" s="48" t="s">
-        <v>32</v>
-      </c>
-      <c r="F64" s="48" t="s">
-        <v>32</v>
-      </c>
-      <c r="G64" s="48" t="s">
-        <v>32</v>
-      </c>
-      <c r="H64" s="48" t="s">
-        <v>32</v>
-      </c>
-      <c r="I64" s="48" t="s">
-        <v>32</v>
-      </c>
-      <c r="J64" s="48" t="s">
-        <v>32</v>
-      </c>
-      <c r="K64" s="48" t="s">
-        <v>32</v>
-      </c>
-      <c r="L64" s="48" t="s">
-        <v>32</v>
-      </c>
-      <c r="M64" s="48" t="s">
-        <v>32</v>
-      </c>
-      <c r="N64" s="48" t="s">
-        <v>280</v>
-      </c>
-      <c r="O64" s="48" t="s">
-        <v>32</v>
-      </c>
-      <c r="P64" s="48" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q64" s="48" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="65" s="45" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="42" t="s">
+      <c r="E64" s="49" t="s">
+        <v>32</v>
+      </c>
+      <c r="F64" s="49" t="s">
+        <v>32</v>
+      </c>
+      <c r="G64" s="49" t="s">
+        <v>32</v>
+      </c>
+      <c r="H64" s="49" t="s">
+        <v>32</v>
+      </c>
+      <c r="I64" s="49" t="s">
+        <v>32</v>
+      </c>
+      <c r="J64" s="49" t="s">
+        <v>32</v>
+      </c>
+      <c r="K64" s="49" t="s">
+        <v>32</v>
+      </c>
+      <c r="L64" s="49" t="s">
+        <v>32</v>
+      </c>
+      <c r="M64" s="49" t="s">
+        <v>32</v>
+      </c>
+      <c r="N64" s="49" t="s">
         <v>281</v>
       </c>
-      <c r="B65" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="C65" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="D65" s="43" t="s">
+      <c r="O64" s="49" t="s">
+        <v>32</v>
+      </c>
+      <c r="P64" s="49" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q64" s="49" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="65" s="46" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="43" t="s">
+        <v>282</v>
+      </c>
+      <c r="B65" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="C65" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="D65" s="44" t="s">
         <v>154</v>
       </c>
-      <c r="E65" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="F65" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="G65" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="H65" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="I65" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="J65" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="K65" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="L65" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="M65" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="N65" s="44" t="s">
-        <v>282</v>
-      </c>
-      <c r="O65" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="P65" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q65" s="43" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="66" s="45" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="42" t="s">
+      <c r="E65" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="F65" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="G65" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="H65" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="I65" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="J65" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="K65" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="L65" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="M65" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="N65" s="45" t="s">
         <v>283</v>
       </c>
-      <c r="B66" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="C66" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="D66" s="43" t="s">
+      <c r="O65" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="P65" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q65" s="44" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="66" s="46" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="43" t="s">
+        <v>284</v>
+      </c>
+      <c r="B66" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="C66" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="D66" s="44" t="s">
         <v>160</v>
       </c>
-      <c r="E66" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="F66" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="G66" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="H66" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="I66" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="J66" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="K66" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="L66" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="M66" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="N66" s="44" t="s">
-        <v>284</v>
-      </c>
-      <c r="O66" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="P66" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q66" s="43" t="s">
+      <c r="E66" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="F66" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="G66" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="H66" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="I66" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="J66" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="K66" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="L66" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="M66" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="N66" s="45" t="s">
+        <v>285</v>
+      </c>
+      <c r="O66" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="P66" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q66" s="44" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="5" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B67" s="6" t="s">
         <v>32</v>
@@ -5286,7 +5296,7 @@
         <v>32</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="E67" s="6" t="s">
         <v>32</v>
@@ -5316,10 +5326,10 @@
         <v>32</v>
       </c>
       <c r="N67" s="6" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="O67" s="6" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="P67" s="6" t="s">
         <v>32</v>
@@ -5330,7 +5340,7 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="5" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B68" s="6" t="s">
         <v>32</v>
@@ -5369,10 +5379,10 @@
         <v>32</v>
       </c>
       <c r="N68" s="6" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="O68" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="P68" s="6" t="s">
         <v>32</v>
@@ -5383,10 +5393,10 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="5" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C69" s="6" t="s">
         <v>32</v>
@@ -5422,7 +5432,7 @@
         <v>156</v>
       </c>
       <c r="N69" s="6" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="O69" s="6" t="s">
         <v>32</v>
@@ -5436,10 +5446,10 @@
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="5" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C70" s="6" t="s">
         <v>32</v>
@@ -5475,7 +5485,7 @@
         <v>32</v>
       </c>
       <c r="N70" s="6" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="O70" s="6" t="s">
         <v>32</v>
@@ -5489,10 +5499,10 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="5" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C71" s="6" t="s">
         <v>32</v>
@@ -5528,10 +5538,10 @@
         <v>32</v>
       </c>
       <c r="N71" s="6" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="O71" s="6" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="P71" s="6" t="s">
         <v>32</v>
@@ -5542,10 +5552,10 @@
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="5" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="C72" s="6" t="s">
         <v>32</v>
@@ -5581,7 +5591,7 @@
         <v>32</v>
       </c>
       <c r="N72" s="6" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="O72" s="6" t="s">
         <v>158</v>
@@ -5595,10 +5605,10 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="5" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C73" s="6" t="s">
         <v>32</v>
@@ -5634,7 +5644,7 @@
         <v>32</v>
       </c>
       <c r="N73" s="6" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="O73" s="6" t="s">
         <v>164</v>
@@ -5646,486 +5656,486 @@
         <v>32</v>
       </c>
     </row>
-    <row r="74" s="45" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="42" t="s">
-        <v>305</v>
-      </c>
-      <c r="B74" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="C74" s="43" t="s">
+    <row r="74" s="46" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="43" t="s">
+        <v>306</v>
+      </c>
+      <c r="B74" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="C74" s="44" t="s">
         <v>104</v>
       </c>
-      <c r="D74" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="E74" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="F74" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="G74" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="H74" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="I74" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="J74" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="K74" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="L74" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="M74" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="N74" s="44" t="s">
-        <v>306</v>
-      </c>
-      <c r="O74" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="P74" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q74" s="43" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="75" s="45" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="42" t="s">
+      <c r="D74" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="E74" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="F74" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="G74" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="H74" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="I74" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="J74" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="K74" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="L74" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="M74" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="N74" s="45" t="s">
         <v>307</v>
       </c>
-      <c r="B75" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="C75" s="43" t="s">
+      <c r="O74" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="P74" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q74" s="44" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="75" s="46" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="43" t="s">
+        <v>308</v>
+      </c>
+      <c r="B75" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="C75" s="44" t="s">
         <v>77</v>
       </c>
-      <c r="D75" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="E75" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="F75" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="G75" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="H75" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="I75" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="J75" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="K75" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="L75" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="M75" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="N75" s="44" t="s">
-        <v>308</v>
-      </c>
-      <c r="O75" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="P75" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q75" s="43" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="76" s="45" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="42" t="s">
+      <c r="D75" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="E75" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="F75" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="G75" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="H75" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="I75" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="J75" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="K75" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="L75" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="M75" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="N75" s="45" t="s">
         <v>309</v>
       </c>
-      <c r="B76" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="C76" s="43" t="s">
+      <c r="O75" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="P75" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q75" s="44" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="76" s="46" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="43" t="s">
+        <v>310</v>
+      </c>
+      <c r="B76" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="C76" s="44" t="s">
         <v>84</v>
       </c>
-      <c r="D76" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="E76" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="F76" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="G76" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="H76" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="I76" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="J76" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="K76" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="L76" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="M76" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="N76" s="44" t="s">
-        <v>310</v>
-      </c>
-      <c r="O76" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="P76" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q76" s="43" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="77" s="45" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="42" t="s">
+      <c r="D76" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="E76" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="F76" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="G76" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="H76" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="I76" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="J76" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="K76" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="L76" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="M76" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="N76" s="45" t="s">
         <v>311</v>
       </c>
-      <c r="B77" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="C77" s="43" t="s">
+      <c r="O76" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="P76" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q76" s="44" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="77" s="46" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="43" t="s">
+        <v>312</v>
+      </c>
+      <c r="B77" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="C77" s="44" t="s">
         <v>117</v>
       </c>
-      <c r="D77" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="E77" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="F77" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="G77" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="H77" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="I77" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="J77" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="K77" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="L77" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="M77" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="N77" s="44" t="s">
-        <v>312</v>
-      </c>
-      <c r="O77" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="P77" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q77" s="43" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="78" s="45" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="42" t="s">
+      <c r="D77" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="E77" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="F77" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="G77" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="H77" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="I77" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="J77" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="K77" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="L77" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="M77" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="N77" s="45" t="s">
         <v>313</v>
       </c>
-      <c r="B78" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="C78" s="43" t="s">
+      <c r="O77" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="P77" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q77" s="44" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="78" s="46" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="43" t="s">
+        <v>314</v>
+      </c>
+      <c r="B78" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="C78" s="44" t="s">
         <v>89</v>
       </c>
-      <c r="D78" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="E78" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="F78" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="G78" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="H78" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="I78" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="J78" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="K78" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="L78" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="M78" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="N78" s="44" t="s">
-        <v>314</v>
-      </c>
-      <c r="O78" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="P78" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q78" s="43" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="79" s="45" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="42" t="s">
+      <c r="D78" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="E78" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="F78" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="G78" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="H78" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="I78" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="J78" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="K78" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="L78" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="M78" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="N78" s="45" t="s">
         <v>315</v>
       </c>
-      <c r="B79" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="C79" s="43" t="s">
+      <c r="O78" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="P78" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q78" s="44" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="79" s="46" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="43" t="s">
+        <v>316</v>
+      </c>
+      <c r="B79" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="C79" s="44" t="s">
         <v>123</v>
       </c>
-      <c r="D79" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="E79" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="F79" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="G79" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="H79" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="I79" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="J79" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="K79" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="L79" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="M79" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="N79" s="44" t="s">
-        <v>316</v>
-      </c>
-      <c r="O79" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="P79" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q79" s="43" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="80" s="45" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="42" t="s">
+      <c r="D79" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="E79" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="F79" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="G79" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="H79" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="I79" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="J79" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="K79" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="L79" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="M79" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="N79" s="45" t="s">
         <v>317</v>
       </c>
-      <c r="B80" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="C80" s="43" t="s">
+      <c r="O79" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="P79" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q79" s="44" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="80" s="46" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="43" t="s">
+        <v>318</v>
+      </c>
+      <c r="B80" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="C80" s="44" t="s">
         <v>94</v>
       </c>
-      <c r="D80" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="E80" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="F80" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="G80" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="H80" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="I80" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="J80" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="K80" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="L80" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="M80" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="N80" s="44" t="s">
-        <v>318</v>
-      </c>
-      <c r="O80" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="P80" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q80" s="43" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="81" s="45" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="42" t="s">
+      <c r="D80" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="E80" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="F80" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="G80" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="H80" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="I80" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="J80" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="K80" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="L80" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="M80" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="N80" s="45" t="s">
         <v>319</v>
       </c>
-      <c r="B81" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="C81" s="43" t="s">
+      <c r="O80" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="P80" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q80" s="44" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="81" s="46" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="43" t="s">
+        <v>320</v>
+      </c>
+      <c r="B81" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="C81" s="44" t="s">
         <v>99</v>
       </c>
-      <c r="D81" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="E81" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="F81" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="G81" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="H81" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="I81" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="J81" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="K81" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="L81" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="M81" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="N81" s="44" t="s">
-        <v>320</v>
-      </c>
-      <c r="O81" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="P81" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q81" s="43" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="82" s="45" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="42" t="s">
+      <c r="D81" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="E81" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="F81" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="G81" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="H81" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="I81" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="J81" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="K81" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="L81" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="M81" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="N81" s="45" t="s">
         <v>321</v>
       </c>
-      <c r="B82" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="C82" s="43" t="s">
+      <c r="O81" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="P81" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q81" s="44" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="82" s="46" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="43" t="s">
+        <v>322</v>
+      </c>
+      <c r="B82" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="C82" s="44" t="s">
         <v>70</v>
       </c>
-      <c r="D82" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="E82" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="F82" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="G82" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="H82" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="I82" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="J82" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="K82" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="L82" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="M82" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="N82" s="44" t="s">
-        <v>322</v>
-      </c>
-      <c r="O82" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="P82" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q82" s="43" t="s">
+      <c r="D82" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="E82" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="F82" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="G82" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="H82" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="I82" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="J82" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="K82" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="L82" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="M82" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="N82" s="45" t="s">
+        <v>323</v>
+      </c>
+      <c r="O82" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="P82" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q82" s="44" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="5" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B83" s="6" t="s">
         <v>32</v>
@@ -6164,7 +6174,7 @@
         <v>32</v>
       </c>
       <c r="N83" s="6" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="O83" s="6" t="s">
         <v>32</v>
@@ -6178,7 +6188,7 @@
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="5" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B84" s="6" t="s">
         <v>32</v>
@@ -6217,7 +6227,7 @@
         <v>32</v>
       </c>
       <c r="N84" s="6" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="O84" s="6" t="s">
         <v>32</v>
@@ -6231,7 +6241,7 @@
     </row>
     <row r="85" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="5" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B85" s="6" t="s">
         <v>32</v>
@@ -6270,7 +6280,7 @@
         <v>32</v>
       </c>
       <c r="N85" s="6" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="O85" s="6" t="s">
         <v>32</v>
@@ -6284,7 +6294,7 @@
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B86" s="6" t="s">
         <v>32</v>
@@ -6323,7 +6333,7 @@
         <v>32</v>
       </c>
       <c r="N86" s="6" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="O86" s="6" t="s">
         <v>32</v>
@@ -6337,7 +6347,7 @@
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="5" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B87" s="6" t="s">
         <v>32</v>
@@ -6376,7 +6386,7 @@
         <v>32</v>
       </c>
       <c r="N87" s="6" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="O87" s="6" t="s">
         <v>32</v>
@@ -6390,7 +6400,7 @@
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="5" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="B88" s="6" t="s">
         <v>32</v>
@@ -6429,7 +6439,7 @@
         <v>32</v>
       </c>
       <c r="N88" s="6" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O88" s="6" t="s">
         <v>32</v>
@@ -6443,7 +6453,7 @@
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="5" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B89" s="6" t="s">
         <v>32</v>
@@ -6480,7 +6490,7 @@
         <v>32</v>
       </c>
       <c r="N89" s="6" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="O89" s="6" t="s">
         <v>32</v>
@@ -6494,7 +6504,7 @@
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="5" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B90" s="6" t="s">
         <v>32</v>
@@ -6531,7 +6541,7 @@
         <v>32</v>
       </c>
       <c r="N90" s="6" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="O90" s="6" t="s">
         <v>32</v>
@@ -6545,7 +6555,7 @@
     </row>
     <row r="91" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="5" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="B91" s="6" t="s">
         <v>32</v>
@@ -6584,7 +6594,7 @@
         <v>32</v>
       </c>
       <c r="N91" s="7" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="O91" s="6" t="s">
         <v>32</v>
@@ -6598,7 +6608,7 @@
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="5" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B92" s="6" t="s">
         <v>32</v>
@@ -6637,7 +6647,7 @@
         <v>32</v>
       </c>
       <c r="N92" s="6" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="O92" s="6" t="s">
         <v>32</v>
@@ -6651,7 +6661,7 @@
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="5" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B93" s="6" t="s">
         <v>32</v>
@@ -6690,7 +6700,7 @@
         <v>32</v>
       </c>
       <c r="N93" s="6" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="O93" s="6" t="s">
         <v>32</v>
@@ -6704,7 +6714,7 @@
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="5" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B94" s="6" t="s">
         <v>32</v>
@@ -6746,7 +6756,7 @@
         <v>32</v>
       </c>
       <c r="O94" s="6" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="P94" s="6" t="s">
         <v>32</v>
@@ -6757,7 +6767,7 @@
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="5" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B95" s="6" t="s">
         <v>32</v>
@@ -6796,7 +6806,7 @@
         <v>32</v>
       </c>
       <c r="N95" s="6" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="O95" s="6" t="s">
         <v>32</v>
@@ -6810,7 +6820,7 @@
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="5" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B96" s="6" t="s">
         <v>32</v>
@@ -6849,7 +6859,7 @@
         <v>32</v>
       </c>
       <c r="N96" s="6" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="O96" s="6" t="s">
         <v>32</v>
@@ -6863,7 +6873,7 @@
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="5" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B97" s="6" t="s">
         <v>32</v>
@@ -6902,7 +6912,7 @@
         <v>32</v>
       </c>
       <c r="N97" s="6" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="O97" s="6" t="s">
         <v>32</v>
@@ -6916,7 +6926,7 @@
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="5" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B98" s="6" t="s">
         <v>32</v>
@@ -6955,7 +6965,7 @@
         <v>32</v>
       </c>
       <c r="N98" s="6" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="O98" s="6" t="s">
         <v>32</v>
@@ -6969,7 +6979,7 @@
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="5" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B99" s="6" t="s">
         <v>32</v>
@@ -7008,7 +7018,7 @@
         <v>32</v>
       </c>
       <c r="N99" s="6" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="O99" s="6" t="s">
         <v>32</v>
@@ -7022,7 +7032,7 @@
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="5" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="B100" s="6" t="s">
         <v>32</v>
@@ -7061,7 +7071,7 @@
         <v>32</v>
       </c>
       <c r="N100" s="6" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="O100" s="6" t="s">
         <v>32</v>
@@ -7075,7 +7085,7 @@
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="5" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="B101" s="6" t="s">
         <v>32</v>
@@ -7114,7 +7124,7 @@
         <v>32</v>
       </c>
       <c r="N101" s="6" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="O101" s="6" t="s">
         <v>32</v>
@@ -7128,7 +7138,7 @@
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="5" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="B102" s="6" t="s">
         <v>32</v>
@@ -7167,7 +7177,7 @@
         <v>32</v>
       </c>
       <c r="N102" s="6" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="O102" s="6" t="s">
         <v>32</v>
@@ -7181,7 +7191,7 @@
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="5" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="B103" s="6" t="s">
         <v>32</v>
@@ -7220,7 +7230,7 @@
         <v>32</v>
       </c>
       <c r="N103" s="6" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="O103" s="6" t="s">
         <v>32</v>
@@ -7234,7 +7244,7 @@
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="5" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B104" s="6" t="s">
         <v>32</v>
@@ -7273,7 +7283,7 @@
         <v>32</v>
       </c>
       <c r="N104" s="6" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="O104" s="6" t="s">
         <v>32</v>
@@ -7287,7 +7297,7 @@
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="5" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="B105" s="6" t="s">
         <v>32</v>
@@ -7326,7 +7336,7 @@
         <v>32</v>
       </c>
       <c r="N105" s="6" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="O105" s="6" t="s">
         <v>32</v>
@@ -7340,7 +7350,7 @@
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="5" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="B106" s="6" t="s">
         <v>32</v>
@@ -7367,7 +7377,7 @@
         <v>32</v>
       </c>
       <c r="J106" s="6" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="K106" s="6" t="s">
         <v>32</v>
@@ -7379,7 +7389,7 @@
         <v>32</v>
       </c>
       <c r="N106" s="6" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="O106" s="6" t="s">
         <v>32</v>
@@ -7393,7 +7403,7 @@
     </row>
     <row r="107" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="5" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="B107" s="6" t="s">
         <v>32</v>
@@ -7420,7 +7430,7 @@
         <v>32</v>
       </c>
       <c r="J107" s="7" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="K107" s="6" t="s">
         <v>32</v>
@@ -7446,7 +7456,7 @@
     </row>
     <row r="108" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="5" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="B108" s="6" t="s">
         <v>32</v>
@@ -7473,7 +7483,7 @@
         <v>32</v>
       </c>
       <c r="J108" s="6" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="K108" s="6" t="s">
         <v>32</v>
@@ -7485,7 +7495,7 @@
         <v>32</v>
       </c>
       <c r="N108" s="7" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="O108" s="6" t="s">
         <v>32</v>
@@ -7499,7 +7509,7 @@
     </row>
     <row r="109" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="5" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="B109" s="6" t="s">
         <v>32</v>
@@ -7538,7 +7548,7 @@
         <v>32</v>
       </c>
       <c r="N109" s="7" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="O109" s="6" t="s">
         <v>32</v>
@@ -7552,7 +7562,7 @@
     </row>
     <row r="110" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="5" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="B110" s="6" t="s">
         <v>32</v>
@@ -7588,10 +7598,10 @@
         <v>32</v>
       </c>
       <c r="M110" s="7" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="N110" s="7" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="O110" s="6" t="s">
         <v>32</v>
@@ -7605,7 +7615,7 @@
     </row>
     <row r="111" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="5" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="B111" s="6" t="s">
         <v>32</v>
@@ -7632,7 +7642,7 @@
         <v>32</v>
       </c>
       <c r="J111" s="7" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="K111" s="6" t="s">
         <v>32</v>
@@ -7644,7 +7654,7 @@
         <v>32</v>
       </c>
       <c r="N111" s="6" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="O111" s="6" t="s">
         <v>32</v>
@@ -7658,7 +7668,7 @@
     </row>
     <row r="112" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="5" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="B112" s="6" t="s">
         <v>32</v>
@@ -7685,7 +7695,7 @@
         <v>32</v>
       </c>
       <c r="J112" s="6" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K112" s="6" t="s">
         <v>32</v>
@@ -7694,10 +7704,10 @@
         <v>32</v>
       </c>
       <c r="M112" s="7" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="N112" s="6" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="O112" s="6" t="s">
         <v>32</v>
@@ -7711,7 +7721,7 @@
     </row>
     <row r="113" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="5" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="B113" s="6" t="s">
         <v>32</v>
@@ -7738,7 +7748,7 @@
         <v>32</v>
       </c>
       <c r="J113" s="6" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="K113" s="6" t="s">
         <v>32</v>
@@ -7750,7 +7760,7 @@
         <v>186</v>
       </c>
       <c r="N113" s="6" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="O113" s="6" t="s">
         <v>32</v>
@@ -7764,7 +7774,7 @@
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="5" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="B114" s="6" t="s">
         <v>32</v>
@@ -7791,7 +7801,7 @@
         <v>32</v>
       </c>
       <c r="J114" s="6" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K114" s="6" t="s">
         <v>32</v>
@@ -7806,7 +7816,7 @@
         <v>32</v>
       </c>
       <c r="O114" s="6" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="P114" s="6" t="s">
         <v>32</v>
@@ -7817,7 +7827,7 @@
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="5" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B115" s="6" t="s">
         <v>32</v>
@@ -7870,7 +7880,7 @@
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="5" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="B116" s="6" t="s">
         <v>32</v>
@@ -7923,7 +7933,7 @@
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="5" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="B117" s="6" t="s">
         <v>32</v>
@@ -7976,7 +7986,7 @@
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="5" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="B118" s="6" t="s">
         <v>32</v>
@@ -8029,7 +8039,7 @@
     </row>
     <row r="119" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="5" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B119" s="6" t="s">
         <v>32</v>
@@ -8062,7 +8072,7 @@
         <v>32</v>
       </c>
       <c r="L119" s="7" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="M119" s="6" t="s">
         <v>32</v>
@@ -8082,7 +8092,7 @@
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="5" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B120" s="6" t="s">
         <v>32</v>
@@ -8135,7 +8145,7 @@
     </row>
     <row r="121" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="5" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B121" s="6" t="s">
         <v>32</v>
@@ -8188,7 +8198,7 @@
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="5" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B122" s="6" t="s">
         <v>32</v>
@@ -8241,7 +8251,7 @@
     </row>
     <row r="123" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="5" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="B123" s="6" t="s">
         <v>32</v>
@@ -8256,7 +8266,7 @@
         <v>32</v>
       </c>
       <c r="F123" s="6" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="G123" s="6" t="s">
         <v>32</v>
@@ -8294,7 +8304,7 @@
     </row>
     <row r="124" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="5" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="B124" s="6" t="s">
         <v>32</v>
@@ -8347,7 +8357,7 @@
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="5" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B125" s="6" t="s">
         <v>32</v>
@@ -8356,7 +8366,7 @@
         <v>32</v>
       </c>
       <c r="D125" s="6" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="E125" s="6" t="s">
         <v>32</v>
@@ -8400,7 +8410,7 @@
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="5" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B126" s="6" t="s">
         <v>32</v>
@@ -8409,7 +8419,7 @@
         <v>32</v>
       </c>
       <c r="D126" s="6" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="E126" s="6" t="s">
         <v>32</v>
@@ -8442,7 +8452,7 @@
         <v>32</v>
       </c>
       <c r="O126" s="6" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="P126" s="6" t="s">
         <v>32</v>
@@ -8453,7 +8463,7 @@
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="5" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="B127" s="6" t="s">
         <v>32</v>
@@ -8462,7 +8472,7 @@
         <v>32</v>
       </c>
       <c r="D127" s="6" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="E127" s="6" t="s">
         <v>32</v>
@@ -8495,7 +8505,7 @@
         <v>32</v>
       </c>
       <c r="O127" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="P127" s="6" t="s">
         <v>32</v>
@@ -8506,7 +8516,7 @@
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="5" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B128" s="6" t="s">
         <v>32</v>
@@ -8545,7 +8555,7 @@
       <c r="N128" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="O128" s="50" t="s">
+      <c r="O128" s="51" t="s">
         <v>32</v>
       </c>
       <c r="P128" s="6" t="s">
@@ -8557,7 +8567,7 @@
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="5" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="B129" s="6" t="s">
         <v>32</v>
@@ -8599,7 +8609,7 @@
         <v>32</v>
       </c>
       <c r="O129" s="6" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="P129" s="6" t="s">
         <v>32</v>
@@ -8610,7 +8620,7 @@
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="5" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="B130" s="6" t="s">
         <v>32</v>
@@ -8652,7 +8662,7 @@
         <v>32</v>
       </c>
       <c r="O130" s="6" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="P130" s="6" t="s">
         <v>32</v>
@@ -8663,7 +8673,7 @@
     </row>
     <row r="131" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="5" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="B131" s="6" t="s">
         <v>32</v>
@@ -8672,7 +8682,7 @@
         <v>32</v>
       </c>
       <c r="D131" s="6" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="E131" s="6" t="s">
         <v>32</v>
@@ -8705,7 +8715,7 @@
         <v>32</v>
       </c>
       <c r="O131" s="6" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="P131" s="6" t="s">
         <v>32</v>
@@ -8716,7 +8726,7 @@
     </row>
     <row r="132" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="5" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B132" s="6" t="s">
         <v>32</v>
@@ -8758,7 +8768,7 @@
         <v>32</v>
       </c>
       <c r="O132" s="6" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="P132" s="6" t="s">
         <v>32</v>
@@ -8769,7 +8779,7 @@
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="5" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="B133" s="6" t="s">
         <v>32</v>
@@ -8781,7 +8791,7 @@
         <v>32</v>
       </c>
       <c r="E133" s="6" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="F133" s="6" t="s">
         <v>32</v>
@@ -8811,7 +8821,7 @@
         <v>32</v>
       </c>
       <c r="O133" s="6" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="P133" s="6" t="s">
         <v>32</v>
@@ -8822,7 +8832,7 @@
     </row>
     <row r="134" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="5" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="B134" s="6" t="s">
         <v>32</v>
@@ -8875,7 +8885,7 @@
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="5" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="B135" s="6" t="s">
         <v>32</v>
@@ -8928,7 +8938,7 @@
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="5" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="B136" s="6" t="s">
         <v>32</v>
@@ -8940,7 +8950,7 @@
         <v>32</v>
       </c>
       <c r="E136" s="6" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="F136" s="6" t="s">
         <v>32</v>
@@ -8981,7 +8991,7 @@
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="5" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="B137" s="6" t="s">
         <v>32</v>
@@ -8993,7 +9003,7 @@
         <v>32</v>
       </c>
       <c r="E137" s="6" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="F137" s="6" t="s">
         <v>32</v>
@@ -9034,7 +9044,7 @@
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="5" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B138" s="6" t="s">
         <v>32</v>
@@ -9046,7 +9056,7 @@
         <v>32</v>
       </c>
       <c r="E138" s="6" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="F138" s="6" t="s">
         <v>32</v>
@@ -9087,7 +9097,7 @@
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="5" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="B139" s="6" t="s">
         <v>32</v>
@@ -9140,7 +9150,7 @@
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="5" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="B140" s="6" t="s">
         <v>32</v>
@@ -9193,7 +9203,7 @@
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="5" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="B141" s="6" t="s">
         <v>32</v>
@@ -9246,7 +9256,7 @@
     </row>
     <row r="142" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="5" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="B142" s="6" t="s">
         <v>32</v>
@@ -9279,7 +9289,7 @@
         <v>32</v>
       </c>
       <c r="L142" s="7" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="M142" s="6" t="s">
         <v>32</v>

</xml_diff>